<commit_message>
Adjusted constraint penalty function
There was an issue with using an Inf multiplication
</commit_message>
<xml_diff>
--- a/Engineering_Optimization/Sim3_Results.xlsx
+++ b/Engineering_Optimization/Sim3_Results.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omarelsewify/Google Drive/MS MechEng/AA222 Engineering Design Optimisation/Final_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omarelsewify/Documents/GitHub/Past-Projects/Engineering_Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6CDD85-4EC7-D744-93EC-F0B3176581EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFAE46B-7F24-C04C-B7C5-3BA9CF1C4DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LARGE_SET" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Simulation Mode</t>
   </si>
@@ -65,7 +66,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +86,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -107,12 +115,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59996337778862885"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,30 +137,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,21 +478,2095 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="113" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.6640625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" style="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="11">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C2" s="11">
+        <v>10</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.52</v>
+      </c>
+      <c r="G2" s="13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H2" s="13">
+        <v>4.37</v>
+      </c>
+      <c r="I2" s="13">
+        <f t="shared" ref="I2:I33" si="0">SUM(E2:H2)</f>
+        <v>9.1499999999999986</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>3</v>
+      </c>
+      <c r="B3" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C3" s="11">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.52</v>
+      </c>
+      <c r="G3" s="13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H3" s="13">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="I3" s="13">
+        <f t="shared" si="0"/>
+        <v>9.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C4" s="11">
+        <v>10</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.59</v>
+      </c>
+      <c r="G4" s="13">
+        <v>4.08</v>
+      </c>
+      <c r="H4" s="13">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="I4" s="13">
+        <f t="shared" si="0"/>
+        <v>9.0100000000000016</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C5" s="11">
+        <v>10</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0.19</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="G5" s="13">
+        <v>4.07</v>
+      </c>
+      <c r="H5" s="13">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="I5" s="13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
+        <v>3</v>
+      </c>
+      <c r="B6" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C6" s="11">
+        <v>10</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="G6" s="13">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H6" s="13">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="I6" s="13">
+        <f t="shared" si="0"/>
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="11">
+        <v>3</v>
+      </c>
+      <c r="B7" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C7" s="11">
+        <v>10</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.78</v>
+      </c>
+      <c r="G7" s="13">
+        <v>4.05</v>
+      </c>
+      <c r="H7" s="13">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I7" s="13">
+        <f t="shared" si="0"/>
+        <v>9.1199999999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="11">
+        <v>3</v>
+      </c>
+      <c r="B8" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C8" s="11">
+        <v>10</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0.96</v>
+      </c>
+      <c r="G8" s="13">
+        <v>4</v>
+      </c>
+      <c r="H8" s="13">
+        <v>4.16</v>
+      </c>
+      <c r="I8" s="13">
+        <f t="shared" si="0"/>
+        <v>9.2800000000000011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
+        <v>3</v>
+      </c>
+      <c r="B9" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C9" s="11">
+        <v>10</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F9" s="11">
+        <v>1.04</v>
+      </c>
+      <c r="G9" s="13">
+        <v>3.97</v>
+      </c>
+      <c r="H9" s="13">
+        <v>4.16</v>
+      </c>
+      <c r="I9" s="13">
+        <f t="shared" si="0"/>
+        <v>9.32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
+        <v>3</v>
+      </c>
+      <c r="B10" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C10" s="11">
+        <v>10</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F10" s="11">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G10" s="13">
+        <v>3.97</v>
+      </c>
+      <c r="H10" s="13">
+        <v>4.16</v>
+      </c>
+      <c r="I10" s="13">
+        <f t="shared" si="0"/>
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="11">
+        <v>3</v>
+      </c>
+      <c r="B11" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C11" s="11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0.09</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F11" s="11">
+        <v>1.23</v>
+      </c>
+      <c r="G11" s="13">
+        <v>3.92</v>
+      </c>
+      <c r="H11" s="13">
+        <v>4.16</v>
+      </c>
+      <c r="I11" s="13">
+        <f t="shared" si="0"/>
+        <v>9.4600000000000009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>3</v>
+      </c>
+      <c r="B12" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C12" s="11">
+        <v>10</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0.08</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1.35</v>
+      </c>
+      <c r="G12" s="13">
+        <v>3.9</v>
+      </c>
+      <c r="H12" s="13">
+        <v>4.17</v>
+      </c>
+      <c r="I12" s="13">
+        <f t="shared" si="0"/>
+        <v>9.58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
+        <v>3</v>
+      </c>
+      <c r="B13" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C13" s="11">
+        <v>10</v>
+      </c>
+      <c r="D13" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="F13" s="11">
+        <v>1.51</v>
+      </c>
+      <c r="G13" s="13">
+        <v>3.84</v>
+      </c>
+      <c r="H13" s="13">
+        <v>4.17</v>
+      </c>
+      <c r="I13" s="13">
+        <f t="shared" si="0"/>
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="11">
+        <v>3</v>
+      </c>
+      <c r="B14" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C14" s="11">
+        <v>10</v>
+      </c>
+      <c r="D14" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F14" s="11">
+        <v>1.56</v>
+      </c>
+      <c r="G14" s="13">
+        <v>3.8</v>
+      </c>
+      <c r="H14" s="13">
+        <v>4.18</v>
+      </c>
+      <c r="I14" s="13">
+        <f t="shared" si="0"/>
+        <v>9.69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="11">
+        <v>3</v>
+      </c>
+      <c r="B15" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C15" s="11">
+        <v>10</v>
+      </c>
+      <c r="D15" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F15" s="11">
+        <v>1.61</v>
+      </c>
+      <c r="G15" s="13">
+        <v>3.78</v>
+      </c>
+      <c r="H15" s="13">
+        <v>4.18</v>
+      </c>
+      <c r="I15" s="13">
+        <f t="shared" si="0"/>
+        <v>9.7199999999999989</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="11">
+        <v>3</v>
+      </c>
+      <c r="B16" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C16" s="11">
+        <v>10</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F16" s="11">
+        <v>1.65</v>
+      </c>
+      <c r="G16" s="13">
+        <v>3.78</v>
+      </c>
+      <c r="H16" s="13">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="I16" s="13">
+        <f t="shared" si="0"/>
+        <v>9.77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="11">
+        <v>3</v>
+      </c>
+      <c r="B17" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C17" s="11">
+        <v>10</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="F17" s="11">
+        <v>1.71</v>
+      </c>
+      <c r="G17" s="13">
+        <v>3.77</v>
+      </c>
+      <c r="H17" s="13">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="I17" s="13">
+        <f t="shared" si="0"/>
+        <v>9.83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
+        <v>3</v>
+      </c>
+      <c r="B18" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C18" s="11">
+        <v>9</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E18" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0.73</v>
+      </c>
+      <c r="G18" s="13">
+        <v>4.07</v>
+      </c>
+      <c r="H18" s="13">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I18" s="13">
+        <f t="shared" si="0"/>
+        <v>9.09</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="11">
+        <v>3</v>
+      </c>
+      <c r="B19" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C19" s="11">
+        <v>8.9</v>
+      </c>
+      <c r="D19" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E19" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F19" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="G19" s="13">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H19" s="13">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="I19" s="13">
+        <f t="shared" si="0"/>
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="11">
+        <v>3</v>
+      </c>
+      <c r="B20" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C20" s="11">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D20" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E20" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="G20" s="13">
+        <v>4.05</v>
+      </c>
+      <c r="H20" s="13">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I20" s="13">
+        <f t="shared" si="0"/>
+        <v>9.0799999999999983</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="11">
+        <v>3</v>
+      </c>
+      <c r="B21" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C21" s="11">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D21" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E21" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F21" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="G21" s="13">
+        <v>4.05</v>
+      </c>
+      <c r="H21" s="13">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I21" s="13">
+        <f t="shared" si="0"/>
+        <v>9.0799999999999983</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="11">
+        <v>3</v>
+      </c>
+      <c r="B22" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C22" s="11">
+        <v>8.6</v>
+      </c>
+      <c r="D22" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E22" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F22" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="G22" s="13">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H22" s="13">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="I22" s="13">
+        <f t="shared" si="0"/>
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="11">
+        <v>3</v>
+      </c>
+      <c r="B23" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C23" s="11">
+        <v>8.5</v>
+      </c>
+      <c r="D23" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E23" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="F23" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="G23" s="13">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H23" s="13">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="I23" s="13">
+        <f t="shared" si="0"/>
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="11">
+        <v>3</v>
+      </c>
+      <c r="B24" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C24" s="11">
+        <v>8</v>
+      </c>
+      <c r="D24" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E24" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="F24" s="11">
+        <v>0.73</v>
+      </c>
+      <c r="G24" s="13">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H24" s="13">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I24" s="13">
+        <f t="shared" si="0"/>
+        <v>9.09</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="11">
+        <v>3</v>
+      </c>
+      <c r="B25" s="11">
+        <v>2500</v>
+      </c>
+      <c r="C25" s="11">
+        <v>8.6</v>
+      </c>
+      <c r="D25" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E25" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F25" s="11">
+        <v>0.73</v>
+      </c>
+      <c r="G25" s="13">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H25" s="13">
+        <v>4.13</v>
+      </c>
+      <c r="I25" s="13">
+        <f t="shared" si="0"/>
+        <v>9.07</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="11">
+        <v>3</v>
+      </c>
+      <c r="B26" s="11">
+        <v>2600</v>
+      </c>
+      <c r="C26" s="11">
+        <v>8.6</v>
+      </c>
+      <c r="D26" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E26" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F26" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="G26" s="13">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H26" s="13">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I26" s="13">
+        <f t="shared" si="0"/>
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="11">
+        <v>3</v>
+      </c>
+      <c r="B27" s="11">
+        <v>2700</v>
+      </c>
+      <c r="C27" s="11">
+        <v>8.6</v>
+      </c>
+      <c r="D27" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E27" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F27" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="G27" s="13">
+        <v>4.07</v>
+      </c>
+      <c r="H27" s="13">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="I27" s="13">
+        <f t="shared" si="0"/>
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="11">
+        <v>3</v>
+      </c>
+      <c r="B28" s="11">
+        <v>2800</v>
+      </c>
+      <c r="C28" s="11">
+        <v>8.6</v>
+      </c>
+      <c r="D28" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E28" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F28" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="G28" s="13">
+        <v>4.07</v>
+      </c>
+      <c r="H28" s="13">
+        <v>4.16</v>
+      </c>
+      <c r="I28" s="13">
+        <f t="shared" si="0"/>
+        <v>9.120000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="11">
+        <v>3</v>
+      </c>
+      <c r="B29" s="11">
+        <v>2900</v>
+      </c>
+      <c r="C29" s="11">
+        <v>8.6</v>
+      </c>
+      <c r="D29" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E29" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F29" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="G29" s="13">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H29" s="13">
+        <v>4.16</v>
+      </c>
+      <c r="I29" s="13">
+        <f t="shared" si="0"/>
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="11">
+        <v>3</v>
+      </c>
+      <c r="B30" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C30" s="11">
+        <v>8.6</v>
+      </c>
+      <c r="D30" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E30" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="F30" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="G30" s="13">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H30" s="13">
+        <v>4.13</v>
+      </c>
+      <c r="I30" s="13">
+        <f t="shared" si="0"/>
+        <v>9.09</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="11">
+        <v>3</v>
+      </c>
+      <c r="B31" s="11">
+        <v>3100</v>
+      </c>
+      <c r="C31" s="11">
+        <v>8.6</v>
+      </c>
+      <c r="D31" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="E31" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="F31" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="G31" s="13">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H31" s="13">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I31" s="13">
+        <f t="shared" si="0"/>
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="12">
+        <v>3</v>
+      </c>
+      <c r="B32" s="12">
+        <v>3000</v>
+      </c>
+      <c r="C32" s="12">
+        <v>10</v>
+      </c>
+      <c r="D32" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="E32" s="12">
+        <v>0.16</v>
+      </c>
+      <c r="F32" s="12">
+        <v>0.53</v>
+      </c>
+      <c r="G32" s="10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H32" s="10">
+        <v>4.34</v>
+      </c>
+      <c r="I32" s="10">
+        <f t="shared" si="0"/>
+        <v>9.129999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
+        <v>3</v>
+      </c>
+      <c r="B33" s="7">
+        <v>2575.012769080744</v>
+      </c>
+      <c r="C33" s="7">
+        <v>8.6046942777306548</v>
+      </c>
+      <c r="D33" s="7">
+        <v>0.21985169413219999</v>
+      </c>
+      <c r="E33" s="7">
+        <v>0.15347199724152999</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0.54300859904743692</v>
+      </c>
+      <c r="G33" s="7">
+        <v>4.0878523572471526</v>
+      </c>
+      <c r="H33" s="7">
+        <v>4.2095429499192454</v>
+      </c>
+      <c r="I33" s="7">
+        <f t="shared" si="0"/>
+        <v>8.9938759034553648</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
+        <v>3</v>
+      </c>
+      <c r="B34" s="7">
+        <v>2526.128334832531</v>
+      </c>
+      <c r="C34" s="7">
+        <v>8.4150915229932153</v>
+      </c>
+      <c r="D34" s="7">
+        <v>0.100871075681712</v>
+      </c>
+      <c r="E34" s="7">
+        <v>0.15435361571669581</v>
+      </c>
+      <c r="F34" s="7">
+        <v>1.112368203313566</v>
+      </c>
+      <c r="G34" s="7">
+        <v>3.957596971789247</v>
+      </c>
+      <c r="H34" s="7">
+        <v>4.1613460505515949</v>
+      </c>
+      <c r="I34" s="7">
+        <f t="shared" ref="I34:I65" si="1">SUM(E34:H34)</f>
+        <v>9.3856648413711028</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
+        <v>3</v>
+      </c>
+      <c r="B35" s="7">
+        <v>2740.2069748110812</v>
+      </c>
+      <c r="C35" s="7">
+        <v>8.8269745716912453</v>
+      </c>
+      <c r="D35" s="7">
+        <v>0.27452426207393149</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0.15561332876471551</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0.52757563509200622</v>
+      </c>
+      <c r="G35" s="7">
+        <v>4.095509701324711</v>
+      </c>
+      <c r="H35" s="7">
+        <v>4.3055251098237273</v>
+      </c>
+      <c r="I35" s="7">
+        <f t="shared" si="1"/>
+        <v>9.0842237750051602</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
+        <v>3</v>
+      </c>
+      <c r="B36" s="7">
+        <v>2574.6580638294949</v>
+      </c>
+      <c r="C36" s="7">
+        <v>8.7052126682383122</v>
+      </c>
+      <c r="D36" s="7">
+        <v>0.34032404298640501</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0.15575802849711409</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0.5312522769794108</v>
+      </c>
+      <c r="G36" s="7">
+        <v>4.1081721068970696</v>
+      </c>
+      <c r="H36" s="7">
+        <v>4.4331490954989397</v>
+      </c>
+      <c r="I36" s="7">
+        <f t="shared" si="1"/>
+        <v>9.2283315078725341</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="7">
+        <v>3</v>
+      </c>
+      <c r="B37" s="7">
+        <v>2699.6611869982589</v>
+      </c>
+      <c r="C37" s="7">
+        <v>8.4746168811559954</v>
+      </c>
+      <c r="D37" s="7">
+        <v>0.22701918730162379</v>
+      </c>
+      <c r="E37" s="7">
+        <v>0.15354463475016489</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0.52782013983798848</v>
+      </c>
+      <c r="G37" s="7">
+        <v>4.0788712653452439</v>
+      </c>
+      <c r="H37" s="7">
+        <v>4.2224001336857198</v>
+      </c>
+      <c r="I37" s="7">
+        <f t="shared" si="1"/>
+        <v>8.9826361736191167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="7">
+        <v>3</v>
+      </c>
+      <c r="B38" s="7">
+        <v>2899.9034796453921</v>
+      </c>
+      <c r="C38" s="7">
+        <v>8.9290852359405299</v>
+      </c>
+      <c r="D38" s="7">
+        <v>0.26507857424223452</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0.15587944051560659</v>
+      </c>
+      <c r="F38" s="7">
+        <v>0.52277633944828761</v>
+      </c>
+      <c r="G38" s="7">
+        <v>4.1087200486270117</v>
+      </c>
+      <c r="H38" s="7">
+        <v>4.2971016304803591</v>
+      </c>
+      <c r="I38" s="7">
+        <f t="shared" si="1"/>
+        <v>9.084477459071266</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
+        <v>3</v>
+      </c>
+      <c r="B39" s="7">
+        <v>2959.4983576816339</v>
+      </c>
+      <c r="C39" s="7">
+        <v>9.7372204956274757</v>
+      </c>
+      <c r="D39" s="7">
+        <v>9.0764199564678308E-2</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0.1543135563357711</v>
+      </c>
+      <c r="F39" s="7">
+        <v>1.223863715025105</v>
+      </c>
+      <c r="G39" s="7">
+        <v>3.9227357619527812</v>
+      </c>
+      <c r="H39" s="7">
+        <v>4.1650164934355072</v>
+      </c>
+      <c r="I39" s="7">
+        <f t="shared" si="1"/>
+        <v>9.4659295267491643</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="7">
+        <v>3</v>
+      </c>
+      <c r="B40" s="7">
+        <v>2663.5399817318448</v>
+      </c>
+      <c r="C40" s="7">
+        <v>8.2588118675427964</v>
+      </c>
+      <c r="D40" s="7">
+        <v>0.17130382067289099</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0.15478167869377521</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0.69506498008619122</v>
+      </c>
+      <c r="G40" s="7">
+        <v>4.0850208378916726</v>
+      </c>
+      <c r="H40" s="7">
+        <v>4.1470121576848404</v>
+      </c>
+      <c r="I40" s="7">
+        <f t="shared" si="1"/>
+        <v>9.0818796543564808</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="7">
+        <v>3</v>
+      </c>
+      <c r="B41" s="7">
+        <v>2663.3761150401838</v>
+      </c>
+      <c r="C41" s="7">
+        <v>7.9673185826289448</v>
+      </c>
+      <c r="D41" s="7">
+        <v>0.29403859403955218</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0.15556920072306321</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0.53165338391456984</v>
+      </c>
+      <c r="G41" s="7">
+        <v>4.0937857299872142</v>
+      </c>
+      <c r="H41" s="7">
+        <v>4.3419282761457429</v>
+      </c>
+      <c r="I41" s="7">
+        <f t="shared" si="1"/>
+        <v>9.122936590770589</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="7">
+        <v>3</v>
+      </c>
+      <c r="B42" s="7">
+        <v>2663.3761150401838</v>
+      </c>
+      <c r="C42" s="7">
+        <v>7.9673185826289448</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0.29403859403955218</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0.15394676021032211</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0.51956230902598266</v>
+      </c>
+      <c r="G42" s="7">
+        <v>4.122152795472604</v>
+      </c>
+      <c r="H42" s="7">
+        <v>4.3455936048211043</v>
+      </c>
+      <c r="I42" s="7">
+        <f t="shared" si="1"/>
+        <v>9.1412554695300123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="7">
+        <v>3</v>
+      </c>
+      <c r="B43" s="7">
+        <v>2575.1214264335749</v>
+      </c>
+      <c r="C43" s="7">
+        <v>8.465134289873145</v>
+      </c>
+      <c r="D43" s="7">
+        <v>0.114560741991427</v>
+      </c>
+      <c r="E43" s="7">
+        <v>0.1538665275500582</v>
+      </c>
+      <c r="F43" s="7">
+        <v>1.0025450682873509</v>
+      </c>
+      <c r="G43" s="7">
+        <v>4.0029458060865313</v>
+      </c>
+      <c r="H43" s="7">
+        <v>4.1561865376837908</v>
+      </c>
+      <c r="I43" s="7">
+        <f t="shared" si="1"/>
+        <v>9.315543939607732</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="7">
+        <v>3</v>
+      </c>
+      <c r="B44" s="7">
+        <v>3062.7113048647898</v>
+      </c>
+      <c r="C44" s="7">
+        <v>8.3774346675269982</v>
+      </c>
+      <c r="D44" s="7">
+        <v>0.16144279076772919</v>
+      </c>
+      <c r="E44" s="7">
+        <v>0.15421725580304449</v>
+      </c>
+      <c r="F44" s="7">
+        <v>0.73427045144466252</v>
+      </c>
+      <c r="G44" s="7">
+        <v>4.0501141047394018</v>
+      </c>
+      <c r="H44" s="7">
+        <v>4.1379367994365976</v>
+      </c>
+      <c r="I44" s="7">
+        <f t="shared" si="1"/>
+        <v>9.0765386114237074</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="7">
+        <v>3</v>
+      </c>
+      <c r="B45" s="7">
+        <v>2812.807544823635</v>
+      </c>
+      <c r="C45" s="7">
+        <v>9.8203848135959522</v>
+      </c>
+      <c r="D45" s="7">
+        <v>8.0617173893371794E-2</v>
+      </c>
+      <c r="E45" s="7">
+        <v>0.15448362864315959</v>
+      </c>
+      <c r="F45" s="7">
+        <v>1.3439169875270029</v>
+      </c>
+      <c r="G45" s="7">
+        <v>3.8841270141930782</v>
+      </c>
+      <c r="H45" s="7">
+        <v>4.1680045761836269</v>
+      </c>
+      <c r="I45" s="7">
+        <f t="shared" si="1"/>
+        <v>9.5505322065468672</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="7">
+        <v>3</v>
+      </c>
+      <c r="B46" s="7">
+        <v>2812.7999314329272</v>
+      </c>
+      <c r="C46" s="7">
+        <v>9.8255921257462528</v>
+      </c>
+      <c r="D46" s="7">
+        <v>7.8769505838609866E-2</v>
+      </c>
+      <c r="E46" s="7">
+        <v>0.15408058504749769</v>
+      </c>
+      <c r="F46" s="7">
+        <v>1.3706173574795051</v>
+      </c>
+      <c r="G46" s="7">
+        <v>3.872323367050289</v>
+      </c>
+      <c r="H46" s="7">
+        <v>4.1660935062750548</v>
+      </c>
+      <c r="I46" s="7">
+        <f t="shared" si="1"/>
+        <v>9.563114815852348</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="7">
+        <v>3</v>
+      </c>
+      <c r="B47" s="7">
+        <v>2835.843246355656</v>
+      </c>
+      <c r="C47" s="7">
+        <v>9.0753783445345757</v>
+      </c>
+      <c r="D47" s="7">
+        <v>0.10640193176729509</v>
+      </c>
+      <c r="E47" s="7">
+        <v>0.1538269948427482</v>
+      </c>
+      <c r="F47" s="7">
+        <v>1.070125579761823</v>
+      </c>
+      <c r="G47" s="7">
+        <v>3.97646796486237</v>
+      </c>
+      <c r="H47" s="7">
+        <v>4.1736579435811683</v>
+      </c>
+      <c r="I47" s="7">
+        <f t="shared" si="1"/>
+        <v>9.374078483048109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="7">
+        <v>3</v>
+      </c>
+      <c r="B48" s="7">
+        <v>2959.4960249617902</v>
+      </c>
+      <c r="C48" s="7">
+        <v>9.7388191294077906</v>
+      </c>
+      <c r="D48" s="7">
+        <v>9.2015048793461285E-2</v>
+      </c>
+      <c r="E48" s="7">
+        <v>0.1547498409337085</v>
+      </c>
+      <c r="F48" s="7">
+        <v>1.2021094991635899</v>
+      </c>
+      <c r="G48" s="7">
+        <v>3.9302242417081561</v>
+      </c>
+      <c r="H48" s="7">
+        <v>4.1561262847043894</v>
+      </c>
+      <c r="I48" s="7">
+        <f t="shared" si="1"/>
+        <v>9.443209866509843</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="7">
+        <v>3</v>
+      </c>
+      <c r="B49" s="7">
+        <v>2500.0053861945398</v>
+      </c>
+      <c r="C49" s="7">
+        <v>8.5935489450269831</v>
+      </c>
+      <c r="D49" s="7">
+        <v>0.43811020182944421</v>
+      </c>
+      <c r="E49" s="7">
+        <v>0.15546223937990941</v>
+      </c>
+      <c r="F49" s="7">
+        <v>0.52252921420228704</v>
+      </c>
+      <c r="G49" s="7">
+        <v>4.103292169391743</v>
+      </c>
+      <c r="H49" s="7">
+        <v>4.6731146021021592</v>
+      </c>
+      <c r="I49" s="7">
+        <f t="shared" si="1"/>
+        <v>9.4543982250760976</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="7">
+        <v>3</v>
+      </c>
+      <c r="B50" s="7">
+        <v>2911.3493520550142</v>
+      </c>
+      <c r="C50" s="7">
+        <v>9.7043807252801901</v>
+      </c>
+      <c r="D50" s="7">
+        <v>0.1482426969216859</v>
+      </c>
+      <c r="E50" s="7">
+        <v>0.15351445932543839</v>
+      </c>
+      <c r="F50" s="7">
+        <v>0.78813214581279123</v>
+      </c>
+      <c r="G50" s="7">
+        <v>4.0649443023961069</v>
+      </c>
+      <c r="H50" s="7">
+        <v>4.1414409860817774</v>
+      </c>
+      <c r="I50" s="7">
+        <f t="shared" si="1"/>
+        <v>9.148031893616114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="7">
+        <v>3</v>
+      </c>
+      <c r="B51" s="7">
+        <v>2911.3493520550142</v>
+      </c>
+      <c r="C51" s="7">
+        <v>9.7043807252801901</v>
+      </c>
+      <c r="D51" s="7">
+        <v>0.1482426969216859</v>
+      </c>
+      <c r="E51" s="7">
+        <v>0.1545690425937836</v>
+      </c>
+      <c r="F51" s="7">
+        <v>0.79096066559657707</v>
+      </c>
+      <c r="G51" s="7">
+        <v>4.0740994835370019</v>
+      </c>
+      <c r="H51" s="7">
+        <v>4.1371687845100924</v>
+      </c>
+      <c r="I51" s="7">
+        <f t="shared" si="1"/>
+        <v>9.1567979762374563</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="7">
+        <v>3</v>
+      </c>
+      <c r="B52" s="7">
+        <v>2879.849219097955</v>
+      </c>
+      <c r="C52" s="7">
+        <v>8.4326056199707047</v>
+      </c>
+      <c r="D52" s="7">
+        <v>0.36013021674185652</v>
+      </c>
+      <c r="E52" s="7">
+        <v>0.15241785672183991</v>
+      </c>
+      <c r="F52" s="7">
+        <v>0.51875369709541497</v>
+      </c>
+      <c r="G52" s="7">
+        <v>4.1171296193236246</v>
+      </c>
+      <c r="H52" s="7">
+        <v>4.471603085382263</v>
+      </c>
+      <c r="I52" s="7">
+        <f t="shared" si="1"/>
+        <v>9.259904258523143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="7">
+        <v>3</v>
+      </c>
+      <c r="B53" s="7">
+        <v>2742.119576626309</v>
+      </c>
+      <c r="C53" s="7">
+        <v>8.5574235030369277</v>
+      </c>
+      <c r="D53" s="7">
+        <v>0.19030618811858649</v>
+      </c>
+      <c r="E53" s="7">
+        <v>0.15424705397202559</v>
+      </c>
+      <c r="F53" s="7">
+        <v>0.6248081866796289</v>
+      </c>
+      <c r="G53" s="7">
+        <v>4.0856811802138324</v>
+      </c>
+      <c r="H53" s="7">
+        <v>4.1390365125606428</v>
+      </c>
+      <c r="I53" s="7">
+        <f t="shared" si="1"/>
+        <v>9.0037729334261307</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="7">
+        <v>3</v>
+      </c>
+      <c r="B54" s="7">
+        <v>2977.4152281434858</v>
+      </c>
+      <c r="C54" s="7">
+        <v>9.0225668062510742</v>
+      </c>
+      <c r="D54" s="7">
+        <v>0.23824914613661721</v>
+      </c>
+      <c r="E54" s="7">
+        <v>0.15297762341926391</v>
+      </c>
+      <c r="F54" s="7">
+        <v>0.52332219282021519</v>
+      </c>
+      <c r="G54" s="7">
+        <v>4.0913846266337606</v>
+      </c>
+      <c r="H54" s="7">
+        <v>4.2281142627348274</v>
+      </c>
+      <c r="I54" s="7">
+        <f t="shared" si="1"/>
+        <v>8.9957987056080668</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="7">
+        <v>3</v>
+      </c>
+      <c r="B55" s="7">
+        <v>2984.6565356916208</v>
+      </c>
+      <c r="C55" s="7">
+        <v>9.2592286878137156</v>
+      </c>
+      <c r="D55" s="7">
+        <v>0.38186103084864831</v>
+      </c>
+      <c r="E55" s="7">
+        <v>0.1542965307002975</v>
+      </c>
+      <c r="F55" s="7">
+        <v>0.53029751151550242</v>
+      </c>
+      <c r="G55" s="7">
+        <v>4.1023291400997532</v>
+      </c>
+      <c r="H55" s="7">
+        <v>4.5401366172963256</v>
+      </c>
+      <c r="I55" s="7">
+        <f t="shared" si="1"/>
+        <v>9.3270597996118774</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="7">
+        <v>3</v>
+      </c>
+      <c r="B56" s="7">
+        <v>2711.792871502169</v>
+      </c>
+      <c r="C56" s="7">
+        <v>9.2822497069522729</v>
+      </c>
+      <c r="D56" s="7">
+        <v>0.17870138311117201</v>
+      </c>
+      <c r="E56" s="7">
+        <v>0.15401988904005751</v>
+      </c>
+      <c r="F56" s="7">
+        <v>0.66240812553909834</v>
+      </c>
+      <c r="G56" s="7">
+        <v>4.0567798095608101</v>
+      </c>
+      <c r="H56" s="7">
+        <v>4.1471767825898853</v>
+      </c>
+      <c r="I56" s="7">
+        <f t="shared" si="1"/>
+        <v>9.0203846067298521</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="7">
+        <v>3</v>
+      </c>
+      <c r="B57" s="7">
+        <v>2877.933601664613</v>
+      </c>
+      <c r="C57" s="7">
+        <v>9.8318288086528405</v>
+      </c>
+      <c r="D57" s="7">
+        <v>0.35302803578631259</v>
+      </c>
+      <c r="E57" s="7">
+        <v>0.15725113264023899</v>
+      </c>
+      <c r="F57" s="7">
+        <v>0.52588798241506396</v>
+      </c>
+      <c r="G57" s="7">
+        <v>4.1005501542654699</v>
+      </c>
+      <c r="H57" s="7">
+        <v>4.4996584847635308</v>
+      </c>
+      <c r="I57" s="7">
+        <f t="shared" si="1"/>
+        <v>9.2833477540843035</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="7">
+        <v>3</v>
+      </c>
+      <c r="B58" s="7">
+        <v>2682.888136523406</v>
+      </c>
+      <c r="C58" s="7">
+        <v>8.1381455037129058</v>
+      </c>
+      <c r="D58" s="7">
+        <v>0.26430165826462149</v>
+      </c>
+      <c r="E58" s="7">
+        <v>0.15415522733661011</v>
+      </c>
+      <c r="F58" s="7">
+        <v>0.52766186249913671</v>
+      </c>
+      <c r="G58" s="7">
+        <v>4.0945739137498087</v>
+      </c>
+      <c r="H58" s="7">
+        <v>4.2747768771330206</v>
+      </c>
+      <c r="I58" s="7">
+        <f t="shared" si="1"/>
+        <v>9.0511678807185767</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="7">
+        <v>3</v>
+      </c>
+      <c r="B59" s="7">
+        <v>2733.3003916589319</v>
+      </c>
+      <c r="C59" s="7">
+        <v>9.4434678957956688</v>
+      </c>
+      <c r="D59" s="7">
+        <v>0.39377433741002588</v>
+      </c>
+      <c r="E59" s="7">
+        <v>0.15511337415934379</v>
+      </c>
+      <c r="F59" s="7">
+        <v>0.52809418130423325</v>
+      </c>
+      <c r="G59" s="7">
+        <v>4.0997212676717476</v>
+      </c>
+      <c r="H59" s="7">
+        <v>4.570589719964409</v>
+      </c>
+      <c r="I59" s="7">
+        <f t="shared" si="1"/>
+        <v>9.3535185430997334</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="7">
+        <v>3</v>
+      </c>
+      <c r="B60" s="7">
+        <v>2567.347060392653</v>
+      </c>
+      <c r="C60" s="7">
+        <v>8.9602482944320148</v>
+      </c>
+      <c r="D60" s="7">
+        <v>0.27605459121150228</v>
+      </c>
+      <c r="E60" s="7">
+        <v>0.1517666150577352</v>
+      </c>
+      <c r="F60" s="7">
+        <v>0.52607237698998732</v>
+      </c>
+      <c r="G60" s="7">
+        <v>4.0975856713130234</v>
+      </c>
+      <c r="H60" s="7">
+        <v>4.3161658623925661</v>
+      </c>
+      <c r="I60" s="7">
+        <f t="shared" si="1"/>
+        <v>9.0915905257533112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="7">
+        <v>3</v>
+      </c>
+      <c r="B61" s="7">
+        <v>2739.420645398985</v>
+      </c>
+      <c r="C61" s="7">
+        <v>9.6014307341190364</v>
+      </c>
+      <c r="D61" s="7">
+        <v>0.13563786210503409</v>
+      </c>
+      <c r="E61" s="7">
+        <v>0.15695384394698569</v>
+      </c>
+      <c r="F61" s="7">
+        <v>0.85745818471793278</v>
+      </c>
+      <c r="G61" s="7">
+        <v>4.033551113037583</v>
+      </c>
+      <c r="H61" s="7">
+        <v>4.1499134703729901</v>
+      </c>
+      <c r="I61" s="7">
+        <f t="shared" si="1"/>
+        <v>9.1978766120754916</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="7">
+        <v>3</v>
+      </c>
+      <c r="B62" s="7">
+        <v>2621.1536760486229</v>
+      </c>
+      <c r="C62" s="7">
+        <v>9.3675113526019622</v>
+      </c>
+      <c r="D62" s="7">
+        <v>0.1598409750012531</v>
+      </c>
+      <c r="E62" s="7">
+        <v>0.15463196072777469</v>
+      </c>
+      <c r="F62" s="7">
+        <v>0.73296078699253719</v>
+      </c>
+      <c r="G62" s="7">
+        <v>4.06896029169003</v>
+      </c>
+      <c r="H62" s="7">
+        <v>4.1472329755117388</v>
+      </c>
+      <c r="I62" s="7">
+        <f t="shared" si="1"/>
+        <v>9.1037860149220808</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="7">
+        <v>3</v>
+      </c>
+      <c r="B63" s="7">
+        <v>2858.4205491602552</v>
+      </c>
+      <c r="C63" s="7">
+        <v>8.6359355802623607</v>
+      </c>
+      <c r="D63" s="7">
+        <v>0.26784415375474813</v>
+      </c>
+      <c r="E63" s="7">
+        <v>0.1528720427247563</v>
+      </c>
+      <c r="F63" s="7">
+        <v>0.52497438463486157</v>
+      </c>
+      <c r="G63" s="7">
+        <v>4.1153750569020424</v>
+      </c>
+      <c r="H63" s="7">
+        <v>4.2889203954926796</v>
+      </c>
+      <c r="I63" s="7">
+        <f t="shared" si="1"/>
+        <v>9.0821418797543387</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="7">
+        <v>3</v>
+      </c>
+      <c r="B64" s="7">
+        <v>3019.4618912440501</v>
+      </c>
+      <c r="C64" s="7">
+        <v>8.8197086101367113</v>
+      </c>
+      <c r="D64" s="7">
+        <v>0.27601066524871198</v>
+      </c>
+      <c r="E64" s="7">
+        <v>0.15247143971122379</v>
+      </c>
+      <c r="F64" s="7">
+        <v>0.52172892956879835</v>
+      </c>
+      <c r="G64" s="7">
+        <v>4.0814606949273147</v>
+      </c>
+      <c r="H64" s="7">
+        <v>4.317735959755101</v>
+      </c>
+      <c r="I64" s="7">
+        <f t="shared" si="1"/>
+        <v>9.0733970239624391</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="7">
+        <v>3</v>
+      </c>
+      <c r="B65" s="7">
+        <v>2951.3914794222019</v>
+      </c>
+      <c r="C65" s="7">
+        <v>9.898037498654821</v>
+      </c>
+      <c r="D65" s="7">
+        <v>0.39726793612717121</v>
+      </c>
+      <c r="E65" s="7">
+        <v>0.15373387873702599</v>
+      </c>
+      <c r="F65" s="7">
+        <v>0.52261298168191272</v>
+      </c>
+      <c r="G65" s="7">
+        <v>4.1096259356424873</v>
+      </c>
+      <c r="H65" s="7">
+        <v>4.5971360440368869</v>
+      </c>
+      <c r="I65" s="7">
+        <f t="shared" si="1"/>
+        <v>9.3831088400983127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="7">
+        <v>3</v>
+      </c>
+      <c r="B66" s="7">
+        <v>3037.8259830031652</v>
+      </c>
+      <c r="C66" s="7">
+        <v>8.3349344028667893</v>
+      </c>
+      <c r="D66" s="7">
+        <v>0.31939786199108439</v>
+      </c>
+      <c r="E66" s="7">
+        <v>0.1531173154819451</v>
+      </c>
+      <c r="F66" s="7">
+        <v>0.52152144372652609</v>
+      </c>
+      <c r="G66" s="7">
+        <v>4.1063322950309109</v>
+      </c>
+      <c r="H66" s="7">
+        <v>4.4092193004482532</v>
+      </c>
+      <c r="I66" s="7">
+        <f t="shared" ref="I66:I97" si="2">SUM(E66:H66)</f>
+        <v>9.1901903546876351</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="7">
+        <v>3</v>
+      </c>
+      <c r="B67" s="7">
+        <v>3020.555708458352</v>
+      </c>
+      <c r="C67" s="7">
+        <v>8.817736848650922</v>
+      </c>
+      <c r="D67" s="7">
+        <v>0.27622487672345469</v>
+      </c>
+      <c r="E67" s="7">
+        <v>0.1547679165128874</v>
+      </c>
+      <c r="F67" s="7">
+        <v>0.53110213867779121</v>
+      </c>
+      <c r="G67" s="7">
+        <v>4.1053349401179391</v>
+      </c>
+      <c r="H67" s="7">
+        <v>4.2989163361681717</v>
+      </c>
+      <c r="I67" s="7">
+        <f t="shared" si="2"/>
+        <v>9.0901213314767908</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="14">
+        <v>3</v>
+      </c>
+      <c r="B68" s="14">
+        <v>2959.3692508232862</v>
+      </c>
+      <c r="C68" s="14">
+        <v>9.6719975780328884</v>
+      </c>
+      <c r="D68" s="14">
+        <v>8.487795936945644E-2</v>
+      </c>
+      <c r="E68" s="14">
+        <v>0.15254571825197322</v>
+      </c>
+      <c r="F68" s="14">
+        <v>1.2935935504083638</v>
+      </c>
+      <c r="G68" s="14">
+        <v>3.8995108953709723</v>
+      </c>
+      <c r="H68" s="14">
+        <v>4.169266330658604</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>3</v>
+      </c>
+      <c r="B249">
+        <v>2959.3692508232862</v>
+      </c>
+      <c r="C249">
+        <v>9.6719975780328884</v>
+      </c>
+      <c r="D249">
+        <v>8.487795936945644E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I153"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" zoomScale="113" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -502,931 +2599,931 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9">
-        <v>3</v>
-      </c>
-      <c r="B2" s="9">
+      <c r="A2" s="5">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5">
         <v>3000</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="5">
         <v>10</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="5">
         <v>0.3</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="5">
         <v>0.155224474043727</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="5">
         <v>0.51868410562909162</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="6">
         <v>4.0958896830207783</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="6">
         <v>4.3696754134039946</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="6">
         <f t="shared" ref="I2:I33" si="0">SUM(E2:H2)</f>
         <v>9.139473676097591</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
-        <v>3</v>
-      </c>
-      <c r="B3" s="9">
+      <c r="A3" s="5">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
         <v>3000</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="5">
         <v>10</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="5">
         <v>0.25</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="5">
         <v>0.1567381482957268</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="5">
         <v>0.52413613771465872</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="6">
         <v>4.0994731360377186</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="6">
         <v>4.2321821720441752</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="6">
         <f t="shared" si="0"/>
         <v>9.0125295940922783</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
-        <v>3</v>
-      </c>
-      <c r="B4" s="9">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
         <v>3000</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="5">
         <v>10</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="5">
         <v>0.2</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="5">
         <v>0.15420613201077121</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="5">
         <v>0.59421879800252952</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="6">
         <v>4.076212776711043</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="6">
         <v>4.185887121111378</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="6">
         <f t="shared" si="0"/>
         <v>9.010524827835722</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
-        <v>3</v>
-      </c>
-      <c r="B5" s="9">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5">
         <v>3000</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="5">
         <v>10</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="5">
         <v>0.19</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="5">
         <v>0.15284554500552719</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="5">
         <v>0.62705399196775069</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="6">
         <v>4.0704452655988836</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="6">
         <v>4.1515902489480832</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="6">
         <f t="shared" si="0"/>
         <v>9.0019350515202454</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
-        <v>3</v>
-      </c>
-      <c r="B6" s="9">
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
         <v>3000</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="5">
         <v>10</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="5">
         <v>0.16</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="5">
         <v>0.15521586983308061</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="5">
         <v>0.73562985975951456</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="6">
         <v>4.0617291257784292</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="6">
         <v>4.1517147043608391</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="6">
         <f t="shared" si="0"/>
         <v>9.104289559731864</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
-        <v>3</v>
-      </c>
-      <c r="B7" s="9">
+      <c r="A7" s="5">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
         <v>3000</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="5">
         <v>10</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="5">
         <v>0.15</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="5">
         <v>0.15380770455585629</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="5">
         <v>0.78246604735172731</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="6">
         <v>4.0460511483277726</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="6">
         <v>4.1384643846675608</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="6">
         <f t="shared" si="0"/>
         <v>9.1207892849029175</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
-        <v>3</v>
-      </c>
-      <c r="B8" s="9">
+      <c r="A8" s="5">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5">
         <v>3000</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="5">
         <v>10</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="5">
         <v>0.12</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="5">
         <v>0.15557879216872239</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="5">
         <v>0.96039347238331985</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="6">
         <v>3.9966888354483241</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="6">
         <v>4.1572515771930432</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="6">
         <f t="shared" si="0"/>
         <v>9.2699126771934104</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="9">
-        <v>3</v>
-      </c>
-      <c r="B9" s="9">
+      <c r="A9" s="5">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5">
         <v>3000</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="5">
         <v>10</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="5">
         <v>0.11</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="5">
         <v>0.1535026006030876</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="5">
         <v>1.0388917570188081</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="6">
         <v>3.971965778256898</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="6">
         <v>4.1556703952227867</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="6">
         <f t="shared" si="0"/>
         <v>9.3200305311015796</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>3</v>
-      </c>
-      <c r="B10" s="9">
+      <c r="A10" s="5">
+        <v>3</v>
+      </c>
+      <c r="B10" s="5">
         <v>3000</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="5">
         <v>10</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="5">
         <v>0.1</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="5">
         <v>0.15370274898323649</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="5">
         <v>1.121019151301859</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="6">
         <v>3.9745690237190821</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="6">
         <v>4.1592328222280566</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="6">
         <f t="shared" si="0"/>
         <v>9.408523746232234</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
-        <v>3</v>
-      </c>
-      <c r="B11" s="9">
+      <c r="A11" s="5">
+        <v>3</v>
+      </c>
+      <c r="B11" s="5">
         <v>3000</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="5">
         <v>10</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="5">
         <v>0.09</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="5">
         <v>0.154280073895459</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="5">
         <v>1.231968462758563</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="6">
         <v>3.9180797494129629</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="6">
         <v>4.1607782814835517</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="6">
         <f t="shared" si="0"/>
         <v>9.4651065675505368</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>3</v>
-      </c>
-      <c r="B12" s="9">
+      <c r="A12" s="5">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5">
         <v>3000</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="5">
         <v>10</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="5">
         <v>0.08</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="5">
         <v>0.1554060678090739</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="5">
         <v>1.3532981683768031</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="6">
         <v>3.8954723736624781</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="6">
         <v>4.1740483314108099</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="6">
         <f t="shared" si="0"/>
         <v>9.5782249412591653</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>3</v>
-      </c>
-      <c r="B13" s="9">
+      <c r="A13" s="5">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5">
         <v>3000</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="5">
         <v>0.15542626181164421</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="5">
         <v>1.514970588111062</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="6">
         <v>3.8435786460439969</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="6">
         <v>4.1742480907853281</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="6">
         <f t="shared" si="0"/>
         <v>9.6882235867520308</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="9">
-        <v>3</v>
-      </c>
-      <c r="B14" s="9">
+      <c r="A14" s="5">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5">
         <v>3000</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="5">
         <v>10</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="5">
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="5">
         <v>0.15341619526340941</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="5">
         <v>1.556753820736511</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="6">
         <v>3.7996951901565268</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="6">
         <v>4.1778947245189819</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="6">
         <f t="shared" si="0"/>
         <v>9.6877599306754298</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>3</v>
-      </c>
-      <c r="B15" s="9">
+      <c r="A15" s="5">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5">
         <v>3000</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="5">
         <v>10</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="5">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="5">
         <v>0.1522971761920241</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="5">
         <v>1.6106606013580791</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="6">
         <v>3.7849320788577989</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="6">
         <v>4.1796915859467019</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="6">
         <f t="shared" si="0"/>
         <v>9.7275814423546052</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>3</v>
-      </c>
-      <c r="B16" s="9">
+      <c r="A16" s="5">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5">
         <v>3000</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="5">
         <v>10</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="5">
         <v>6.25E-2</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="5">
         <v>0.15426664869060061</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="5">
         <v>1.654283502923283</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="6">
         <v>3.7791644571794292</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="6">
         <v>4.1880678792663391</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="6">
         <f t="shared" si="0"/>
         <v>9.7757824880596509</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>3</v>
-      </c>
-      <c r="B17" s="9">
+      <c r="A17" s="5">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5">
         <v>3000</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="5">
         <v>10</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="5">
         <v>0.06</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="5">
         <v>0.15516651074421781</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="5">
         <v>1.707687502546696</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="6">
         <v>3.7653951446013361</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="6">
         <v>4.1906939994793317</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="6">
         <f t="shared" si="0"/>
         <v>9.8189431573715815</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>3</v>
-      </c>
-      <c r="B18" s="9">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
+      <c r="B18" s="5">
         <v>3000</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="5">
         <v>9</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="5">
         <v>0.16</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="5">
         <v>0.15379337660495979</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="5">
         <v>0.73433443791726294</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="6">
         <v>4.0693420360242936</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18" s="6">
         <v>4.1429635199634998</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="6">
         <f t="shared" si="0"/>
         <v>9.1004333705100162</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
-        <v>3</v>
-      </c>
-      <c r="B19" s="9">
+      <c r="A19" s="5">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5">
         <v>3000</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="5">
         <v>8.9</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="5">
         <v>0.16</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="5">
         <v>0.15484405567321519</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="5">
         <v>0.73774339574239356</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="6">
         <v>4.0592594620766569</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H19" s="6">
         <v>4.1512436057936739</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="6">
         <f t="shared" si="0"/>
         <v>9.1030905192859386</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="9">
-        <v>3</v>
-      </c>
-      <c r="B20" s="9">
+      <c r="A20" s="5">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5">
         <v>3000</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="5">
         <v>8.8000000000000007</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="5">
         <v>0.16</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="5">
         <v>0.15387973843526501</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="5">
         <v>0.73837422830465371</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="6">
         <v>4.0482521367940052</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="6">
         <v>4.1404657198962749</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="6">
         <f t="shared" si="0"/>
         <v>9.0809718234301986</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="9">
-        <v>3</v>
-      </c>
-      <c r="B21" s="9">
+      <c r="A21" s="5">
+        <v>3</v>
+      </c>
+      <c r="B21" s="5">
         <v>3000</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="5">
         <v>8.6999999999999993</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="5">
         <v>0.16</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="5">
         <v>0.15499228035089799</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="5">
         <v>0.735798935897364</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="6">
         <v>4.0522449071692881</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21" s="6">
         <v>4.1411898131973119</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="6">
         <f t="shared" si="0"/>
         <v>9.0842259366148621</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="9">
-        <v>3</v>
-      </c>
-      <c r="B22" s="9">
+      <c r="A22" s="5">
+        <v>3</v>
+      </c>
+      <c r="B22" s="5">
         <v>3000</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="5">
         <v>8.6</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="5">
         <v>0.16</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="5">
         <v>0.15451744762234901</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="5">
         <v>0.73556460688318914</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="6">
         <v>4.0563853496339188</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22" s="6">
         <v>4.151907385191997</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="6">
         <f t="shared" si="0"/>
         <v>9.098374789331455</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="9">
-        <v>3</v>
-      </c>
-      <c r="B23" s="9">
+      <c r="A23" s="5">
+        <v>3</v>
+      </c>
+      <c r="B23" s="5">
         <v>3000</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="5">
         <v>8.5</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="5">
         <v>0.16</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="5">
         <v>0.1560413398136235</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="5">
         <v>0.73874248204088122</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23" s="6">
         <v>4.060190847436818</v>
       </c>
-      <c r="H23" s="10">
+      <c r="H23" s="6">
         <v>4.1478131291691689</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="6">
         <f t="shared" si="0"/>
         <v>9.1027877984604917</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="9">
-        <v>3</v>
-      </c>
-      <c r="B24" s="9">
+      <c r="A24" s="5">
+        <v>3</v>
+      </c>
+      <c r="B24" s="5">
         <v>3000</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="5">
         <v>8</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="5">
         <v>0.16</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="5">
         <v>0.15535104531255381</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="5">
         <v>0.73374417015929616</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24" s="6">
         <v>4.0633969676277184</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="6">
         <v>4.1402484801420423</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="6">
         <f t="shared" si="0"/>
         <v>9.0927406632416101</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="9">
-        <v>3</v>
-      </c>
-      <c r="B25" s="9">
+      <c r="A25" s="5">
+        <v>3</v>
+      </c>
+      <c r="B25" s="5">
         <v>2500</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="5">
         <v>8.6</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="5">
         <v>0.16</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="5">
         <v>0.1532764712057697</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="5">
         <v>0.73401817425287597</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="6">
         <v>4.0618541124290557</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25" s="6">
         <v>4.133645248169608</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="6">
         <f t="shared" si="0"/>
         <v>9.0827940060573091</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="9">
-        <v>3</v>
-      </c>
-      <c r="B26" s="9">
+      <c r="A26" s="5">
+        <v>3</v>
+      </c>
+      <c r="B26" s="5">
         <v>2600</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="5">
         <v>8.6</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="5">
         <v>0.16</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="5">
         <v>0.15218830252151391</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="5">
         <v>0.74659681991696036</v>
       </c>
-      <c r="G26" s="10">
+      <c r="G26" s="6">
         <v>4.0598254706394279</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26" s="6">
         <v>4.1365139041640981</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26" s="6">
         <f t="shared" si="0"/>
         <v>9.0951244972420007</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="9">
-        <v>3</v>
-      </c>
-      <c r="B27" s="9">
+      <c r="A27" s="5">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5">
         <v>2700</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="5">
         <v>8.6</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="5">
         <v>0.16</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="5">
         <v>0.1518838350488883</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="5">
         <v>0.73639567750370105</v>
       </c>
-      <c r="G27" s="10">
+      <c r="G27" s="6">
         <v>4.0654562749149923</v>
       </c>
-      <c r="H27" s="10">
+      <c r="H27" s="6">
         <v>4.1546984028644678</v>
       </c>
-      <c r="I27" s="10">
+      <c r="I27" s="6">
         <f t="shared" si="0"/>
         <v>9.1084341903320496</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="9">
-        <v>3</v>
-      </c>
-      <c r="B28" s="9">
+      <c r="A28" s="5">
+        <v>3</v>
+      </c>
+      <c r="B28" s="5">
         <v>2800</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="5">
         <v>8.6</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="5">
         <v>0.16</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="5">
         <v>0.15378164855065821</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="5">
         <v>0.73734326249242166</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="6">
         <v>4.0659664557461088</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H28" s="6">
         <v>4.1553125526198178</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28" s="6">
         <f t="shared" si="0"/>
         <v>9.1124039194090063</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="9">
-        <v>3</v>
-      </c>
-      <c r="B29" s="9">
+      <c r="A29" s="5">
+        <v>3</v>
+      </c>
+      <c r="B29" s="5">
         <v>2900</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="5">
         <v>8.6</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="5">
         <v>0.16</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="5">
         <v>0.15296627069402149</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="5">
         <v>0.73819829782842472</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="6">
         <v>4.0569624593137643</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H29" s="6">
         <v>4.1552067668710446</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I29" s="6">
         <f t="shared" si="0"/>
         <v>9.1033337947072539</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="9">
-        <v>3</v>
-      </c>
-      <c r="B30" s="9">
+      <c r="A30" s="5">
+        <v>3</v>
+      </c>
+      <c r="B30" s="5">
         <v>3000</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="5">
         <v>8.6</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="5">
         <v>0.16</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="5">
         <v>0.15538684189326329</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="5">
         <v>0.74010506473170334</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G30" s="6">
         <v>4.0579964108399924</v>
       </c>
-      <c r="H30" s="10">
+      <c r="H30" s="6">
         <v>4.1348355703760884</v>
       </c>
-      <c r="I30" s="10">
+      <c r="I30" s="6">
         <f t="shared" si="0"/>
         <v>9.0883238878410477</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="9">
-        <v>3</v>
-      </c>
-      <c r="B31" s="9">
+      <c r="A31" s="5">
+        <v>3</v>
+      </c>
+      <c r="B31" s="5">
         <v>3100</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="5">
         <v>8.6</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="5">
         <v>0.16</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="5">
         <v>0.15521853230945709</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31" s="5">
         <v>0.73586263857068879</v>
       </c>
-      <c r="G31" s="10">
+      <c r="G31" s="6">
         <v>4.0636215055443428</v>
       </c>
-      <c r="H31" s="10">
+      <c r="H31" s="6">
         <v>4.1353534432440453</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I31" s="6">
         <f t="shared" si="0"/>
         <v>9.0900561196685352</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4">
-        <v>3</v>
-      </c>
-      <c r="B32" s="4">
+    <row r="32" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="12">
+        <v>3</v>
+      </c>
+      <c r="B32" s="12">
         <v>3000</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="12">
         <v>10</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="12">
         <v>0.3</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="12">
         <v>0.15525102322819009</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="12">
         <v>0.53035584455315909</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="3">
         <v>4.1014142987509903</v>
       </c>
-      <c r="H32" s="5">
+      <c r="H32" s="3">
         <v>4.3377933616965887</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I32" s="6">
         <f t="shared" si="0"/>
         <v>9.1248145282289279</v>
       </c>
@@ -2302,145 +4399,731 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="8">
-        <v>3</v>
-      </c>
-      <c r="B62" s="8">
+      <c r="A62" s="7">
+        <v>3</v>
+      </c>
+      <c r="B62" s="7">
         <v>2621.1536760486229</v>
       </c>
-      <c r="C62" s="8">
+      <c r="C62" s="7">
         <v>9.3675113526019622</v>
       </c>
-      <c r="D62" s="8">
+      <c r="D62" s="7">
         <v>0.1598409750012531</v>
       </c>
-      <c r="E62" s="8">
+      <c r="E62" s="7">
         <v>0.15463196072777469</v>
       </c>
-      <c r="F62" s="8">
+      <c r="F62" s="7">
         <v>0.73296078699253719</v>
       </c>
-      <c r="G62" s="8">
+      <c r="G62" s="7">
         <v>4.06896029169003</v>
       </c>
-      <c r="H62" s="8">
+      <c r="H62" s="7">
         <v>4.1472329755117388</v>
       </c>
-      <c r="I62" s="8">
+      <c r="I62" s="7">
         <f t="shared" si="1"/>
         <v>9.1037860149220808</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="8">
-        <v>3</v>
-      </c>
-      <c r="B63" s="8">
+      <c r="A63" s="7">
+        <v>3</v>
+      </c>
+      <c r="B63" s="7">
         <v>2858.4205491602552</v>
       </c>
-      <c r="C63" s="8">
+      <c r="C63" s="7">
         <v>8.6359355802623607</v>
       </c>
-      <c r="D63" s="8">
+      <c r="D63" s="7">
         <v>0.26784415375474813</v>
       </c>
-      <c r="E63" s="8">
+      <c r="E63" s="7">
         <v>0.1528720427247563</v>
       </c>
-      <c r="F63" s="8">
+      <c r="F63" s="7">
         <v>0.52497438463486157</v>
       </c>
-      <c r="G63" s="8">
+      <c r="G63" s="7">
         <v>4.1153750569020424</v>
       </c>
-      <c r="H63" s="8">
+      <c r="H63" s="7">
         <v>4.2889203954926796</v>
       </c>
-      <c r="I63" s="8">
+      <c r="I63" s="7">
         <f t="shared" si="1"/>
         <v>9.0821418797543387</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="8">
-        <v>3</v>
-      </c>
-      <c r="B64" s="8">
+      <c r="A64" s="7">
+        <v>3</v>
+      </c>
+      <c r="B64" s="7">
         <v>3019.4618912440501</v>
       </c>
-      <c r="C64" s="8">
+      <c r="C64" s="7">
         <v>8.8197086101367113</v>
       </c>
-      <c r="D64" s="8">
+      <c r="D64" s="7">
         <v>0.27601066524871198</v>
       </c>
-      <c r="E64" s="8">
+      <c r="E64" s="7">
         <v>0.15247143971122379</v>
       </c>
-      <c r="F64" s="8">
+      <c r="F64" s="7">
         <v>0.52172892956879835</v>
       </c>
-      <c r="G64" s="8">
+      <c r="G64" s="7">
         <v>4.0814606949273147</v>
       </c>
-      <c r="H64" s="8">
+      <c r="H64" s="7">
         <v>4.317735959755101</v>
       </c>
-      <c r="I64" s="8">
+      <c r="I64" s="7">
         <f t="shared" si="1"/>
         <v>9.0733970239624391</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>3</v>
-      </c>
-      <c r="B65">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="7">
+        <v>3</v>
+      </c>
+      <c r="B65" s="7">
         <v>2951.3914794222019</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="7">
         <v>9.898037498654821</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="7">
         <v>0.39726793612717121</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="7">
         <v>0.15373387873702599</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="7">
         <v>0.52261298168191272</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="7">
         <v>4.1096259356424873</v>
       </c>
-      <c r="H65">
+      <c r="H65" s="7">
         <v>4.5971360440368869</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>3</v>
-      </c>
-      <c r="B66">
+      <c r="I65" s="7">
+        <f t="shared" si="1"/>
+        <v>9.3831088400983127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="7">
+        <v>3</v>
+      </c>
+      <c r="B66" s="7">
         <v>3037.8259830031652</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="7">
         <v>8.3349344028667893</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="7">
         <v>0.31939786199108439</v>
       </c>
-      <c r="E66" s="3">
+      <c r="E66" s="7">
         <v>0.1531173154819451</v>
       </c>
-      <c r="F66" s="3">
+      <c r="F66" s="7">
         <v>0.52152144372652609</v>
       </c>
-      <c r="G66" s="3">
+      <c r="G66" s="7">
         <v>4.1063322950309109</v>
       </c>
-      <c r="H66" s="3">
+      <c r="H66" s="7">
         <v>4.4092193004482532</v>
+      </c>
+      <c r="I66" s="7">
+        <f t="shared" ref="I66:I97" si="2">SUM(E66:H66)</f>
+        <v>9.1901903546876351</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="7">
+        <v>3</v>
+      </c>
+      <c r="B67" s="7">
+        <v>3020.555708458352</v>
+      </c>
+      <c r="C67" s="7">
+        <v>8.817736848650922</v>
+      </c>
+      <c r="D67" s="7">
+        <v>0.27622487672345469</v>
+      </c>
+      <c r="E67" s="7">
+        <v>0.1547679165128874</v>
+      </c>
+      <c r="F67" s="7">
+        <v>0.53110213867779121</v>
+      </c>
+      <c r="G67" s="7">
+        <v>4.1053349401179391</v>
+      </c>
+      <c r="H67" s="7">
+        <v>4.2989163361681717</v>
+      </c>
+      <c r="I67" s="7">
+        <f t="shared" si="2"/>
+        <v>9.0901213314767908</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>2700.4233564017791</v>
+      </c>
+      <c r="C68">
+        <v>8.5185938546033828</v>
+      </c>
+      <c r="D68">
+        <v>0.20288437185451699</v>
+      </c>
+      <c r="E68" s="8">
+        <v>0.1547104355748854</v>
+      </c>
+      <c r="F68" s="8">
+        <v>0.59062446258447121</v>
+      </c>
+      <c r="G68" s="8">
+        <v>4.0919130962562846</v>
+      </c>
+      <c r="H68" s="8">
+        <v>4.1771971241180204</v>
+      </c>
+      <c r="I68" s="7">
+        <f t="shared" si="2"/>
+        <v>9.0144451185336614</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I69" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I70" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I71" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I72" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I73" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I74" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I75" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I76" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I77" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I78" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I79" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I80" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I81" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I82" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I83" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I84" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I85" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I86" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I87" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I88" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I89" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I90" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I91" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I92" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I93" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I94" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I95" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I96" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I97" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I98" s="7">
+        <f t="shared" ref="I98:I129" si="3">SUM(E98:H98)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I99" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I100" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I101" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I102" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I103" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I104" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I105" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I106" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I107" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I108" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I109" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I110" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I111" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I112" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I113" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I114" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I115" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I116" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I117" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I118" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I119" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I120" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I121" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I122" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I123" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I124" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I125" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I126" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I127" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I128" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I129" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I130" s="7">
+        <f t="shared" ref="I130:I161" si="4">SUM(E130:H130)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I131" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I132" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I133" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I134" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I135" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I136" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I137" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I138" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I139" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I140" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I141" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I142" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I143" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I144" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I145" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I146" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I147" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I148" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I149" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I150" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I151" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I152" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>3</v>
+      </c>
+      <c r="B153">
+        <v>2997.7780916562119</v>
+      </c>
+      <c r="C153">
+        <v>9.185878827123874</v>
+      </c>
+      <c r="D153">
+        <v>0.55241584241542085</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added log of of objective function
y_history added
</commit_message>
<xml_diff>
--- a/Engineering_Optimization/Sim3_Results.xlsx
+++ b/Engineering_Optimization/Sim3_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omarelsewify/Documents/GitHub/Past-Projects/Engineering_Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFAE46B-7F24-C04C-B7C5-3BA9CF1C4DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3695365B-8436-5F40-9E8F-DD2D326A83AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -478,17 +478,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I249"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.1640625" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.6640625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="14" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.1640625" style="14" bestFit="1" customWidth="1"/>
@@ -550,7 +550,7 @@
         <v>4.37</v>
       </c>
       <c r="I2" s="13">
-        <f t="shared" ref="I2:I33" si="0">SUM(E2:H2)</f>
+        <f t="shared" ref="I2:I32" si="0">SUM(E2:H2)</f>
         <v>9.1499999999999986</v>
       </c>
     </row>
@@ -1454,1095 +1454,21 @@
         <v>9.129999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="7">
-        <v>3</v>
-      </c>
-      <c r="B33" s="7">
-        <v>2575.012769080744</v>
-      </c>
-      <c r="C33" s="7">
-        <v>8.6046942777306548</v>
-      </c>
-      <c r="D33" s="7">
-        <v>0.21985169413219999</v>
-      </c>
-      <c r="E33" s="7">
-        <v>0.15347199724152999</v>
-      </c>
-      <c r="F33" s="7">
-        <v>0.54300859904743692</v>
-      </c>
-      <c r="G33" s="7">
-        <v>4.0878523572471526</v>
-      </c>
-      <c r="H33" s="7">
-        <v>4.2095429499192454</v>
-      </c>
-      <c r="I33" s="7">
-        <f t="shared" si="0"/>
-        <v>8.9938759034553648</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="7">
-        <v>3</v>
-      </c>
-      <c r="B34" s="7">
-        <v>2526.128334832531</v>
-      </c>
-      <c r="C34" s="7">
-        <v>8.4150915229932153</v>
-      </c>
-      <c r="D34" s="7">
-        <v>0.100871075681712</v>
-      </c>
-      <c r="E34" s="7">
-        <v>0.15435361571669581</v>
-      </c>
-      <c r="F34" s="7">
-        <v>1.112368203313566</v>
-      </c>
-      <c r="G34" s="7">
-        <v>3.957596971789247</v>
-      </c>
-      <c r="H34" s="7">
-        <v>4.1613460505515949</v>
-      </c>
-      <c r="I34" s="7">
-        <f t="shared" ref="I34:I65" si="1">SUM(E34:H34)</f>
-        <v>9.3856648413711028</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
-        <v>3</v>
-      </c>
-      <c r="B35" s="7">
-        <v>2740.2069748110812</v>
-      </c>
-      <c r="C35" s="7">
-        <v>8.8269745716912453</v>
-      </c>
-      <c r="D35" s="7">
-        <v>0.27452426207393149</v>
-      </c>
-      <c r="E35" s="7">
-        <v>0.15561332876471551</v>
-      </c>
-      <c r="F35" s="7">
-        <v>0.52757563509200622</v>
-      </c>
-      <c r="G35" s="7">
-        <v>4.095509701324711</v>
-      </c>
-      <c r="H35" s="7">
-        <v>4.3055251098237273</v>
-      </c>
-      <c r="I35" s="7">
-        <f t="shared" si="1"/>
-        <v>9.0842237750051602</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="7">
-        <v>3</v>
-      </c>
-      <c r="B36" s="7">
-        <v>2574.6580638294949</v>
-      </c>
-      <c r="C36" s="7">
-        <v>8.7052126682383122</v>
-      </c>
-      <c r="D36" s="7">
-        <v>0.34032404298640501</v>
-      </c>
-      <c r="E36" s="7">
-        <v>0.15575802849711409</v>
-      </c>
-      <c r="F36" s="7">
-        <v>0.5312522769794108</v>
-      </c>
-      <c r="G36" s="7">
-        <v>4.1081721068970696</v>
-      </c>
-      <c r="H36" s="7">
-        <v>4.4331490954989397</v>
-      </c>
-      <c r="I36" s="7">
-        <f t="shared" si="1"/>
-        <v>9.2283315078725341</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="7">
-        <v>3</v>
-      </c>
-      <c r="B37" s="7">
-        <v>2699.6611869982589</v>
-      </c>
-      <c r="C37" s="7">
-        <v>8.4746168811559954</v>
-      </c>
-      <c r="D37" s="7">
-        <v>0.22701918730162379</v>
-      </c>
-      <c r="E37" s="7">
-        <v>0.15354463475016489</v>
-      </c>
-      <c r="F37" s="7">
-        <v>0.52782013983798848</v>
-      </c>
-      <c r="G37" s="7">
-        <v>4.0788712653452439</v>
-      </c>
-      <c r="H37" s="7">
-        <v>4.2224001336857198</v>
-      </c>
-      <c r="I37" s="7">
-        <f t="shared" si="1"/>
-        <v>8.9826361736191167</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="7">
-        <v>3</v>
-      </c>
-      <c r="B38" s="7">
-        <v>2899.9034796453921</v>
-      </c>
-      <c r="C38" s="7">
-        <v>8.9290852359405299</v>
-      </c>
-      <c r="D38" s="7">
-        <v>0.26507857424223452</v>
-      </c>
-      <c r="E38" s="7">
-        <v>0.15587944051560659</v>
-      </c>
-      <c r="F38" s="7">
-        <v>0.52277633944828761</v>
-      </c>
-      <c r="G38" s="7">
-        <v>4.1087200486270117</v>
-      </c>
-      <c r="H38" s="7">
-        <v>4.2971016304803591</v>
-      </c>
-      <c r="I38" s="7">
-        <f t="shared" si="1"/>
-        <v>9.084477459071266</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="7">
-        <v>3</v>
-      </c>
-      <c r="B39" s="7">
-        <v>2959.4983576816339</v>
-      </c>
-      <c r="C39" s="7">
-        <v>9.7372204956274757</v>
-      </c>
-      <c r="D39" s="7">
-        <v>9.0764199564678308E-2</v>
-      </c>
-      <c r="E39" s="7">
-        <v>0.1543135563357711</v>
-      </c>
-      <c r="F39" s="7">
-        <v>1.223863715025105</v>
-      </c>
-      <c r="G39" s="7">
-        <v>3.9227357619527812</v>
-      </c>
-      <c r="H39" s="7">
-        <v>4.1650164934355072</v>
-      </c>
-      <c r="I39" s="7">
-        <f t="shared" si="1"/>
-        <v>9.4659295267491643</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="7">
-        <v>3</v>
-      </c>
-      <c r="B40" s="7">
-        <v>2663.5399817318448</v>
-      </c>
-      <c r="C40" s="7">
-        <v>8.2588118675427964</v>
-      </c>
-      <c r="D40" s="7">
-        <v>0.17130382067289099</v>
-      </c>
-      <c r="E40" s="7">
-        <v>0.15478167869377521</v>
-      </c>
-      <c r="F40" s="7">
-        <v>0.69506498008619122</v>
-      </c>
-      <c r="G40" s="7">
-        <v>4.0850208378916726</v>
-      </c>
-      <c r="H40" s="7">
-        <v>4.1470121576848404</v>
-      </c>
-      <c r="I40" s="7">
-        <f t="shared" si="1"/>
-        <v>9.0818796543564808</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="7">
-        <v>3</v>
-      </c>
-      <c r="B41" s="7">
-        <v>2663.3761150401838</v>
-      </c>
-      <c r="C41" s="7">
-        <v>7.9673185826289448</v>
-      </c>
-      <c r="D41" s="7">
-        <v>0.29403859403955218</v>
-      </c>
-      <c r="E41" s="7">
-        <v>0.15556920072306321</v>
-      </c>
-      <c r="F41" s="7">
-        <v>0.53165338391456984</v>
-      </c>
-      <c r="G41" s="7">
-        <v>4.0937857299872142</v>
-      </c>
-      <c r="H41" s="7">
-        <v>4.3419282761457429</v>
-      </c>
-      <c r="I41" s="7">
-        <f t="shared" si="1"/>
-        <v>9.122936590770589</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="7">
-        <v>3</v>
-      </c>
-      <c r="B42" s="7">
-        <v>2663.3761150401838</v>
-      </c>
-      <c r="C42" s="7">
-        <v>7.9673185826289448</v>
-      </c>
-      <c r="D42" s="7">
-        <v>0.29403859403955218</v>
-      </c>
-      <c r="E42" s="7">
-        <v>0.15394676021032211</v>
-      </c>
-      <c r="F42" s="7">
-        <v>0.51956230902598266</v>
-      </c>
-      <c r="G42" s="7">
-        <v>4.122152795472604</v>
-      </c>
-      <c r="H42" s="7">
-        <v>4.3455936048211043</v>
-      </c>
-      <c r="I42" s="7">
-        <f t="shared" si="1"/>
-        <v>9.1412554695300123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="7">
-        <v>3</v>
-      </c>
-      <c r="B43" s="7">
-        <v>2575.1214264335749</v>
-      </c>
-      <c r="C43" s="7">
-        <v>8.465134289873145</v>
-      </c>
-      <c r="D43" s="7">
-        <v>0.114560741991427</v>
-      </c>
-      <c r="E43" s="7">
-        <v>0.1538665275500582</v>
-      </c>
-      <c r="F43" s="7">
-        <v>1.0025450682873509</v>
-      </c>
-      <c r="G43" s="7">
-        <v>4.0029458060865313</v>
-      </c>
-      <c r="H43" s="7">
-        <v>4.1561865376837908</v>
-      </c>
-      <c r="I43" s="7">
-        <f t="shared" si="1"/>
-        <v>9.315543939607732</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="7">
-        <v>3</v>
-      </c>
-      <c r="B44" s="7">
-        <v>3062.7113048647898</v>
-      </c>
-      <c r="C44" s="7">
-        <v>8.3774346675269982</v>
-      </c>
-      <c r="D44" s="7">
-        <v>0.16144279076772919</v>
-      </c>
-      <c r="E44" s="7">
-        <v>0.15421725580304449</v>
-      </c>
-      <c r="F44" s="7">
-        <v>0.73427045144466252</v>
-      </c>
-      <c r="G44" s="7">
-        <v>4.0501141047394018</v>
-      </c>
-      <c r="H44" s="7">
-        <v>4.1379367994365976</v>
-      </c>
-      <c r="I44" s="7">
-        <f t="shared" si="1"/>
-        <v>9.0765386114237074</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="7">
-        <v>3</v>
-      </c>
-      <c r="B45" s="7">
-        <v>2812.807544823635</v>
-      </c>
-      <c r="C45" s="7">
-        <v>9.8203848135959522</v>
-      </c>
-      <c r="D45" s="7">
-        <v>8.0617173893371794E-2</v>
-      </c>
-      <c r="E45" s="7">
-        <v>0.15448362864315959</v>
-      </c>
-      <c r="F45" s="7">
-        <v>1.3439169875270029</v>
-      </c>
-      <c r="G45" s="7">
-        <v>3.8841270141930782</v>
-      </c>
-      <c r="H45" s="7">
-        <v>4.1680045761836269</v>
-      </c>
-      <c r="I45" s="7">
-        <f t="shared" si="1"/>
-        <v>9.5505322065468672</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="7">
-        <v>3</v>
-      </c>
-      <c r="B46" s="7">
-        <v>2812.7999314329272</v>
-      </c>
-      <c r="C46" s="7">
-        <v>9.8255921257462528</v>
-      </c>
-      <c r="D46" s="7">
-        <v>7.8769505838609866E-2</v>
-      </c>
-      <c r="E46" s="7">
-        <v>0.15408058504749769</v>
-      </c>
-      <c r="F46" s="7">
-        <v>1.3706173574795051</v>
-      </c>
-      <c r="G46" s="7">
-        <v>3.872323367050289</v>
-      </c>
-      <c r="H46" s="7">
-        <v>4.1660935062750548</v>
-      </c>
-      <c r="I46" s="7">
-        <f t="shared" si="1"/>
-        <v>9.563114815852348</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="7">
-        <v>3</v>
-      </c>
-      <c r="B47" s="7">
-        <v>2835.843246355656</v>
-      </c>
-      <c r="C47" s="7">
-        <v>9.0753783445345757</v>
-      </c>
-      <c r="D47" s="7">
-        <v>0.10640193176729509</v>
-      </c>
-      <c r="E47" s="7">
-        <v>0.1538269948427482</v>
-      </c>
-      <c r="F47" s="7">
-        <v>1.070125579761823</v>
-      </c>
-      <c r="G47" s="7">
-        <v>3.97646796486237</v>
-      </c>
-      <c r="H47" s="7">
-        <v>4.1736579435811683</v>
-      </c>
-      <c r="I47" s="7">
-        <f t="shared" si="1"/>
-        <v>9.374078483048109</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="7">
-        <v>3</v>
-      </c>
-      <c r="B48" s="7">
-        <v>2959.4960249617902</v>
-      </c>
-      <c r="C48" s="7">
-        <v>9.7388191294077906</v>
-      </c>
-      <c r="D48" s="7">
-        <v>9.2015048793461285E-2</v>
-      </c>
-      <c r="E48" s="7">
-        <v>0.1547498409337085</v>
-      </c>
-      <c r="F48" s="7">
-        <v>1.2021094991635899</v>
-      </c>
-      <c r="G48" s="7">
-        <v>3.9302242417081561</v>
-      </c>
-      <c r="H48" s="7">
-        <v>4.1561262847043894</v>
-      </c>
-      <c r="I48" s="7">
-        <f t="shared" si="1"/>
-        <v>9.443209866509843</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="7">
-        <v>3</v>
-      </c>
-      <c r="B49" s="7">
-        <v>2500.0053861945398</v>
-      </c>
-      <c r="C49" s="7">
-        <v>8.5935489450269831</v>
-      </c>
-      <c r="D49" s="7">
-        <v>0.43811020182944421</v>
-      </c>
-      <c r="E49" s="7">
-        <v>0.15546223937990941</v>
-      </c>
-      <c r="F49" s="7">
-        <v>0.52252921420228704</v>
-      </c>
-      <c r="G49" s="7">
-        <v>4.103292169391743</v>
-      </c>
-      <c r="H49" s="7">
-        <v>4.6731146021021592</v>
-      </c>
-      <c r="I49" s="7">
-        <f t="shared" si="1"/>
-        <v>9.4543982250760976</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="7">
-        <v>3</v>
-      </c>
-      <c r="B50" s="7">
-        <v>2911.3493520550142</v>
-      </c>
-      <c r="C50" s="7">
-        <v>9.7043807252801901</v>
-      </c>
-      <c r="D50" s="7">
-        <v>0.1482426969216859</v>
-      </c>
-      <c r="E50" s="7">
-        <v>0.15351445932543839</v>
-      </c>
-      <c r="F50" s="7">
-        <v>0.78813214581279123</v>
-      </c>
-      <c r="G50" s="7">
-        <v>4.0649443023961069</v>
-      </c>
-      <c r="H50" s="7">
-        <v>4.1414409860817774</v>
-      </c>
-      <c r="I50" s="7">
-        <f t="shared" si="1"/>
-        <v>9.148031893616114</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="7">
-        <v>3</v>
-      </c>
-      <c r="B51" s="7">
-        <v>2911.3493520550142</v>
-      </c>
-      <c r="C51" s="7">
-        <v>9.7043807252801901</v>
-      </c>
-      <c r="D51" s="7">
-        <v>0.1482426969216859</v>
-      </c>
-      <c r="E51" s="7">
-        <v>0.1545690425937836</v>
-      </c>
-      <c r="F51" s="7">
-        <v>0.79096066559657707</v>
-      </c>
-      <c r="G51" s="7">
-        <v>4.0740994835370019</v>
-      </c>
-      <c r="H51" s="7">
-        <v>4.1371687845100924</v>
-      </c>
-      <c r="I51" s="7">
-        <f t="shared" si="1"/>
-        <v>9.1567979762374563</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="7">
-        <v>3</v>
-      </c>
-      <c r="B52" s="7">
-        <v>2879.849219097955</v>
-      </c>
-      <c r="C52" s="7">
-        <v>8.4326056199707047</v>
-      </c>
-      <c r="D52" s="7">
-        <v>0.36013021674185652</v>
-      </c>
-      <c r="E52" s="7">
-        <v>0.15241785672183991</v>
-      </c>
-      <c r="F52" s="7">
-        <v>0.51875369709541497</v>
-      </c>
-      <c r="G52" s="7">
-        <v>4.1171296193236246</v>
-      </c>
-      <c r="H52" s="7">
-        <v>4.471603085382263</v>
-      </c>
-      <c r="I52" s="7">
-        <f t="shared" si="1"/>
-        <v>9.259904258523143</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="7">
-        <v>3</v>
-      </c>
-      <c r="B53" s="7">
-        <v>2742.119576626309</v>
-      </c>
-      <c r="C53" s="7">
-        <v>8.5574235030369277</v>
-      </c>
-      <c r="D53" s="7">
-        <v>0.19030618811858649</v>
-      </c>
-      <c r="E53" s="7">
-        <v>0.15424705397202559</v>
-      </c>
-      <c r="F53" s="7">
-        <v>0.6248081866796289</v>
-      </c>
-      <c r="G53" s="7">
-        <v>4.0856811802138324</v>
-      </c>
-      <c r="H53" s="7">
-        <v>4.1390365125606428</v>
-      </c>
-      <c r="I53" s="7">
-        <f t="shared" si="1"/>
-        <v>9.0037729334261307</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="7">
-        <v>3</v>
-      </c>
-      <c r="B54" s="7">
-        <v>2977.4152281434858</v>
-      </c>
-      <c r="C54" s="7">
-        <v>9.0225668062510742</v>
-      </c>
-      <c r="D54" s="7">
-        <v>0.23824914613661721</v>
-      </c>
-      <c r="E54" s="7">
-        <v>0.15297762341926391</v>
-      </c>
-      <c r="F54" s="7">
-        <v>0.52332219282021519</v>
-      </c>
-      <c r="G54" s="7">
-        <v>4.0913846266337606</v>
-      </c>
-      <c r="H54" s="7">
-        <v>4.2281142627348274</v>
-      </c>
-      <c r="I54" s="7">
-        <f t="shared" si="1"/>
-        <v>8.9957987056080668</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="7">
-        <v>3</v>
-      </c>
-      <c r="B55" s="7">
-        <v>2984.6565356916208</v>
-      </c>
-      <c r="C55" s="7">
-        <v>9.2592286878137156</v>
-      </c>
-      <c r="D55" s="7">
-        <v>0.38186103084864831</v>
-      </c>
-      <c r="E55" s="7">
-        <v>0.1542965307002975</v>
-      </c>
-      <c r="F55" s="7">
-        <v>0.53029751151550242</v>
-      </c>
-      <c r="G55" s="7">
-        <v>4.1023291400997532</v>
-      </c>
-      <c r="H55" s="7">
-        <v>4.5401366172963256</v>
-      </c>
-      <c r="I55" s="7">
-        <f t="shared" si="1"/>
-        <v>9.3270597996118774</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="7">
-        <v>3</v>
-      </c>
-      <c r="B56" s="7">
-        <v>2711.792871502169</v>
-      </c>
-      <c r="C56" s="7">
-        <v>9.2822497069522729</v>
-      </c>
-      <c r="D56" s="7">
-        <v>0.17870138311117201</v>
-      </c>
-      <c r="E56" s="7">
-        <v>0.15401988904005751</v>
-      </c>
-      <c r="F56" s="7">
-        <v>0.66240812553909834</v>
-      </c>
-      <c r="G56" s="7">
-        <v>4.0567798095608101</v>
-      </c>
-      <c r="H56" s="7">
-        <v>4.1471767825898853</v>
-      </c>
-      <c r="I56" s="7">
-        <f t="shared" si="1"/>
-        <v>9.0203846067298521</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="7">
-        <v>3</v>
-      </c>
-      <c r="B57" s="7">
-        <v>2877.933601664613</v>
-      </c>
-      <c r="C57" s="7">
-        <v>9.8318288086528405</v>
-      </c>
-      <c r="D57" s="7">
-        <v>0.35302803578631259</v>
-      </c>
-      <c r="E57" s="7">
-        <v>0.15725113264023899</v>
-      </c>
-      <c r="F57" s="7">
-        <v>0.52588798241506396</v>
-      </c>
-      <c r="G57" s="7">
-        <v>4.1005501542654699</v>
-      </c>
-      <c r="H57" s="7">
-        <v>4.4996584847635308</v>
-      </c>
-      <c r="I57" s="7">
-        <f t="shared" si="1"/>
-        <v>9.2833477540843035</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="7">
-        <v>3</v>
-      </c>
-      <c r="B58" s="7">
-        <v>2682.888136523406</v>
-      </c>
-      <c r="C58" s="7">
-        <v>8.1381455037129058</v>
-      </c>
-      <c r="D58" s="7">
-        <v>0.26430165826462149</v>
-      </c>
-      <c r="E58" s="7">
-        <v>0.15415522733661011</v>
-      </c>
-      <c r="F58" s="7">
-        <v>0.52766186249913671</v>
-      </c>
-      <c r="G58" s="7">
-        <v>4.0945739137498087</v>
-      </c>
-      <c r="H58" s="7">
-        <v>4.2747768771330206</v>
-      </c>
-      <c r="I58" s="7">
-        <f t="shared" si="1"/>
-        <v>9.0511678807185767</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="7">
-        <v>3</v>
-      </c>
-      <c r="B59" s="7">
-        <v>2733.3003916589319</v>
-      </c>
-      <c r="C59" s="7">
-        <v>9.4434678957956688</v>
-      </c>
-      <c r="D59" s="7">
-        <v>0.39377433741002588</v>
-      </c>
-      <c r="E59" s="7">
-        <v>0.15511337415934379</v>
-      </c>
-      <c r="F59" s="7">
-        <v>0.52809418130423325</v>
-      </c>
-      <c r="G59" s="7">
-        <v>4.0997212676717476</v>
-      </c>
-      <c r="H59" s="7">
-        <v>4.570589719964409</v>
-      </c>
-      <c r="I59" s="7">
-        <f t="shared" si="1"/>
-        <v>9.3535185430997334</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="7">
-        <v>3</v>
-      </c>
-      <c r="B60" s="7">
-        <v>2567.347060392653</v>
-      </c>
-      <c r="C60" s="7">
-        <v>8.9602482944320148</v>
-      </c>
-      <c r="D60" s="7">
-        <v>0.27605459121150228</v>
-      </c>
-      <c r="E60" s="7">
-        <v>0.1517666150577352</v>
-      </c>
-      <c r="F60" s="7">
-        <v>0.52607237698998732</v>
-      </c>
-      <c r="G60" s="7">
-        <v>4.0975856713130234</v>
-      </c>
-      <c r="H60" s="7">
-        <v>4.3161658623925661</v>
-      </c>
-      <c r="I60" s="7">
-        <f t="shared" si="1"/>
-        <v>9.0915905257533112</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="7">
-        <v>3</v>
-      </c>
-      <c r="B61" s="7">
-        <v>2739.420645398985</v>
-      </c>
-      <c r="C61" s="7">
-        <v>9.6014307341190364</v>
-      </c>
-      <c r="D61" s="7">
-        <v>0.13563786210503409</v>
-      </c>
-      <c r="E61" s="7">
-        <v>0.15695384394698569</v>
-      </c>
-      <c r="F61" s="7">
-        <v>0.85745818471793278</v>
-      </c>
-      <c r="G61" s="7">
-        <v>4.033551113037583</v>
-      </c>
-      <c r="H61" s="7">
-        <v>4.1499134703729901</v>
-      </c>
-      <c r="I61" s="7">
-        <f t="shared" si="1"/>
-        <v>9.1978766120754916</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="7">
-        <v>3</v>
-      </c>
-      <c r="B62" s="7">
-        <v>2621.1536760486229</v>
-      </c>
-      <c r="C62" s="7">
-        <v>9.3675113526019622</v>
-      </c>
-      <c r="D62" s="7">
-        <v>0.1598409750012531</v>
-      </c>
-      <c r="E62" s="7">
-        <v>0.15463196072777469</v>
-      </c>
-      <c r="F62" s="7">
-        <v>0.73296078699253719</v>
-      </c>
-      <c r="G62" s="7">
-        <v>4.06896029169003</v>
-      </c>
-      <c r="H62" s="7">
-        <v>4.1472329755117388</v>
-      </c>
-      <c r="I62" s="7">
-        <f t="shared" si="1"/>
-        <v>9.1037860149220808</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="7">
-        <v>3</v>
-      </c>
-      <c r="B63" s="7">
-        <v>2858.4205491602552</v>
-      </c>
-      <c r="C63" s="7">
-        <v>8.6359355802623607</v>
-      </c>
-      <c r="D63" s="7">
-        <v>0.26784415375474813</v>
-      </c>
-      <c r="E63" s="7">
-        <v>0.1528720427247563</v>
-      </c>
-      <c r="F63" s="7">
-        <v>0.52497438463486157</v>
-      </c>
-      <c r="G63" s="7">
-        <v>4.1153750569020424</v>
-      </c>
-      <c r="H63" s="7">
-        <v>4.2889203954926796</v>
-      </c>
-      <c r="I63" s="7">
-        <f t="shared" si="1"/>
-        <v>9.0821418797543387</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="7">
-        <v>3</v>
-      </c>
-      <c r="B64" s="7">
-        <v>3019.4618912440501</v>
-      </c>
-      <c r="C64" s="7">
-        <v>8.8197086101367113</v>
-      </c>
-      <c r="D64" s="7">
-        <v>0.27601066524871198</v>
-      </c>
-      <c r="E64" s="7">
-        <v>0.15247143971122379</v>
-      </c>
-      <c r="F64" s="7">
-        <v>0.52172892956879835</v>
-      </c>
-      <c r="G64" s="7">
-        <v>4.0814606949273147</v>
-      </c>
-      <c r="H64" s="7">
-        <v>4.317735959755101</v>
-      </c>
-      <c r="I64" s="7">
-        <f t="shared" si="1"/>
-        <v>9.0733970239624391</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="7">
-        <v>3</v>
-      </c>
-      <c r="B65" s="7">
-        <v>2951.3914794222019</v>
-      </c>
-      <c r="C65" s="7">
-        <v>9.898037498654821</v>
-      </c>
-      <c r="D65" s="7">
-        <v>0.39726793612717121</v>
-      </c>
-      <c r="E65" s="7">
-        <v>0.15373387873702599</v>
-      </c>
-      <c r="F65" s="7">
-        <v>0.52261298168191272</v>
-      </c>
-      <c r="G65" s="7">
-        <v>4.1096259356424873</v>
-      </c>
-      <c r="H65" s="7">
-        <v>4.5971360440368869</v>
-      </c>
-      <c r="I65" s="7">
-        <f t="shared" si="1"/>
-        <v>9.3831088400983127</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="7">
-        <v>3</v>
-      </c>
-      <c r="B66" s="7">
-        <v>3037.8259830031652</v>
-      </c>
-      <c r="C66" s="7">
-        <v>8.3349344028667893</v>
-      </c>
-      <c r="D66" s="7">
-        <v>0.31939786199108439</v>
-      </c>
-      <c r="E66" s="7">
-        <v>0.1531173154819451</v>
-      </c>
-      <c r="F66" s="7">
-        <v>0.52152144372652609</v>
-      </c>
-      <c r="G66" s="7">
-        <v>4.1063322950309109</v>
-      </c>
-      <c r="H66" s="7">
-        <v>4.4092193004482532</v>
-      </c>
-      <c r="I66" s="7">
-        <f t="shared" ref="I66:I97" si="2">SUM(E66:H66)</f>
-        <v>9.1901903546876351</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="7">
-        <v>3</v>
-      </c>
-      <c r="B67" s="7">
-        <v>3020.555708458352</v>
-      </c>
-      <c r="C67" s="7">
-        <v>8.817736848650922</v>
-      </c>
-      <c r="D67" s="7">
-        <v>0.27622487672345469</v>
-      </c>
-      <c r="E67" s="7">
-        <v>0.1547679165128874</v>
-      </c>
-      <c r="F67" s="7">
-        <v>0.53110213867779121</v>
-      </c>
-      <c r="G67" s="7">
-        <v>4.1053349401179391</v>
-      </c>
-      <c r="H67" s="7">
-        <v>4.2989163361681717</v>
-      </c>
-      <c r="I67" s="7">
-        <f t="shared" si="2"/>
-        <v>9.0901213314767908</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="14">
-        <v>3</v>
-      </c>
-      <c r="B68" s="14">
-        <v>2959.3692508232862</v>
-      </c>
-      <c r="C68" s="14">
-        <v>9.6719975780328884</v>
-      </c>
-      <c r="D68" s="14">
-        <v>8.487795936945644E-2</v>
-      </c>
-      <c r="E68" s="14">
-        <v>0.15254571825197322</v>
-      </c>
-      <c r="F68" s="14">
-        <v>1.2935935504083638</v>
-      </c>
-      <c r="G68" s="14">
-        <v>3.8995108953709723</v>
-      </c>
-      <c r="H68" s="14">
-        <v>4.169266330658604</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A249">
-        <v>3</v>
-      </c>
-      <c r="B249">
-        <v>2959.3692508232862</v>
-      </c>
-      <c r="C249">
-        <v>9.6719975780328884</v>
-      </c>
-      <c r="D249">
-        <v>8.487795936945644E-2</v>
-      </c>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2553,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I153"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="113" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:I67"/>
+    <sheetView topLeftCell="A54" zoomScale="113" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4583,47 +3509,119 @@
         <v>3</v>
       </c>
       <c r="B68">
-        <v>2700.4233564017791</v>
+        <v>2959.3692508232862</v>
       </c>
       <c r="C68">
-        <v>8.5185938546033828</v>
+        <v>9.6719975780328884</v>
       </c>
       <c r="D68">
-        <v>0.20288437185451699</v>
-      </c>
-      <c r="E68" s="8">
-        <v>0.1547104355748854</v>
-      </c>
-      <c r="F68" s="8">
-        <v>0.59062446258447121</v>
-      </c>
-      <c r="G68" s="8">
-        <v>4.0919130962562846</v>
-      </c>
-      <c r="H68" s="8">
-        <v>4.1771971241180204</v>
+        <v>8.487795936945644E-2</v>
+      </c>
+      <c r="E68">
+        <v>0.15254571825197319</v>
+      </c>
+      <c r="F68">
+        <v>1.293593550408364</v>
+      </c>
+      <c r="G68">
+        <v>3.8995108953709718</v>
+      </c>
+      <c r="H68">
+        <v>4.169266330658604</v>
       </c>
       <c r="I68" s="7">
         <f t="shared" si="2"/>
-        <v>9.0144451185336614</v>
+        <v>9.5149164946899134</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>3</v>
+      </c>
+      <c r="B69">
+        <v>2959.3692508232862</v>
+      </c>
+      <c r="C69">
+        <v>9.6719975780328884</v>
+      </c>
+      <c r="D69">
+        <v>8.487795936945644E-2</v>
+      </c>
+      <c r="E69">
+        <v>0.1518574139965376</v>
+      </c>
+      <c r="F69">
+        <v>1.292588882838851</v>
+      </c>
+      <c r="G69">
+        <v>3.905469395961235</v>
+      </c>
+      <c r="H69">
+        <v>4.1610423864597648</v>
+      </c>
       <c r="I69" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.5109580792563886</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>3</v>
+      </c>
+      <c r="B70">
+        <v>2663.854526081539</v>
+      </c>
+      <c r="C70">
+        <v>8.1634615925622764</v>
+      </c>
+      <c r="D70">
+        <v>0.21188195901679549</v>
+      </c>
+      <c r="E70">
+        <v>0.15272497612817021</v>
+      </c>
+      <c r="F70">
+        <v>0.56484611218110192</v>
+      </c>
+      <c r="G70">
+        <v>4.079119281209727</v>
+      </c>
+      <c r="H70">
+        <v>4.190969855812118</v>
+      </c>
       <c r="I70" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.9876602253311173</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>3</v>
+      </c>
+      <c r="B71">
+        <v>2663.854526081539</v>
+      </c>
+      <c r="C71">
+        <v>8.1634615925622764</v>
+      </c>
+      <c r="D71">
+        <v>0.21188195901679549</v>
+      </c>
+      <c r="E71">
+        <v>0.15368086210007059</v>
+      </c>
+      <c r="F71">
+        <v>0.57322509211792294</v>
+      </c>
+      <c r="G71">
+        <v>4.081890679078743</v>
+      </c>
+      <c r="H71">
+        <v>4.1989808873526462</v>
+      </c>
       <c r="I71" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.007777520649384</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Introduced weights to the objective function
</commit_message>
<xml_diff>
--- a/Engineering_Optimization/Sim3_Results.xlsx
+++ b/Engineering_Optimization/Sim3_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omarelsewify/Documents/GitHub/Past-Projects/Engineering_Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3695365B-8436-5F40-9E8F-DD2D326A83AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E7E0C9-CC39-A543-A5AD-134CD611CEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Simulation Mode</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>METRIC</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,6 +179,10 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -521,7 +528,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -529,59 +536,59 @@
         <v>3</v>
       </c>
       <c r="B2" s="11">
-        <v>3000</v>
+        <v>2500</v>
       </c>
       <c r="C2" s="11">
-        <v>10</v>
+        <v>8.6</v>
       </c>
       <c r="D2" s="11">
-        <v>0.3</v>
+        <v>0.16</v>
       </c>
       <c r="E2" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.73</v>
+      </c>
+      <c r="G2" s="13">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H2" s="13">
+        <v>4.13</v>
+      </c>
+      <c r="I2" s="13">
+        <f>(MAX(E2-0.2,0))^2+(MAX(F2-0.75,0))^2+(MAX(G2-4,0))^2 +(MAX(H2-4,0))^2</f>
+        <v>2.0499999999999925E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="15">
+        <v>3</v>
+      </c>
+      <c r="B3" s="15">
+        <v>3000</v>
+      </c>
+      <c r="C3" s="15">
+        <v>8.6</v>
+      </c>
+      <c r="D3" s="15">
         <v>0.16</v>
       </c>
-      <c r="F2" s="11">
-        <v>0.52</v>
-      </c>
-      <c r="G2" s="13">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="H2" s="13">
-        <v>4.37</v>
-      </c>
-      <c r="I2" s="13">
-        <f t="shared" ref="I2:I32" si="0">SUM(E2:H2)</f>
-        <v>9.1499999999999986</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="11">
-        <v>3</v>
-      </c>
-      <c r="B3" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C3" s="11">
-        <v>10</v>
-      </c>
-      <c r="D3" s="11">
-        <v>0.25</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="E3" s="15">
         <v>0.16</v>
       </c>
-      <c r="F3" s="11">
-        <v>0.52</v>
-      </c>
-      <c r="G3" s="13">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="H3" s="13">
-        <v>4.2300000000000004</v>
+      <c r="F3" s="15">
+        <v>0.74</v>
+      </c>
+      <c r="G3" s="16">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H3" s="16">
+        <v>4.13</v>
       </c>
       <c r="I3" s="13">
-        <f t="shared" si="0"/>
-        <v>9.01</v>
+        <f>(MAX(E3-0.2,0))^2+(MAX(F3-0.75,0))^2+(MAX(G3-4,0))^2 +(MAX(H3-4,0))^2</f>
+        <v>2.0499999999999925E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -592,26 +599,26 @@
         <v>3000</v>
       </c>
       <c r="C4" s="11">
-        <v>10</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="D4" s="11">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="E4" s="11">
         <v>0.15</v>
       </c>
       <c r="F4" s="11">
-        <v>0.59</v>
+        <v>0.74</v>
       </c>
       <c r="G4" s="13">
-        <v>4.08</v>
+        <v>4.05</v>
       </c>
       <c r="H4" s="13">
-        <v>4.1900000000000004</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="I4" s="13">
-        <f t="shared" si="0"/>
-        <v>9.0100000000000016</v>
+        <f>(MAX(E4-0.2,0))^2+(MAX(F4-0.75,0))^2+(MAX(G4-4,0))^2 +(MAX(H4-4,0))^2</f>
+        <v>2.2099999999999891E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -622,26 +629,26 @@
         <v>3000</v>
       </c>
       <c r="C5" s="11">
-        <v>10</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D5" s="11">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="E5" s="11">
         <v>0.15</v>
       </c>
       <c r="F5" s="11">
-        <v>0.63</v>
+        <v>0.74</v>
       </c>
       <c r="G5" s="13">
-        <v>4.07</v>
+        <v>4.05</v>
       </c>
       <c r="H5" s="13">
-        <v>4.1500000000000004</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="I5" s="13">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f>(MAX(E5-0.2,0))^2+(MAX(F5-0.75,0))^2+(MAX(G5-4,0))^2 +(MAX(H5-4,0))^2</f>
+        <v>2.2099999999999891E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -655,23 +662,23 @@
         <v>10</v>
       </c>
       <c r="D6" s="11">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="E6" s="11">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F6" s="11">
-        <v>0.74</v>
+        <v>0.78</v>
       </c>
       <c r="G6" s="13">
-        <v>4.0599999999999996</v>
+        <v>4.05</v>
       </c>
       <c r="H6" s="13">
-        <v>4.1500000000000004</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="I6" s="13">
-        <f t="shared" si="0"/>
-        <v>9.11</v>
+        <f>(MAX(E6-0.2,0))^2+(MAX(F6-0.75,0))^2+(MAX(G6-4,0))^2 +(MAX(H6-4,0))^2</f>
+        <v>2.2999999999999892E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -682,26 +689,26 @@
         <v>3000</v>
       </c>
       <c r="C7" s="11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" s="11">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="E7" s="11">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F7" s="11">
-        <v>0.78</v>
+        <v>0.73</v>
       </c>
       <c r="G7" s="13">
-        <v>4.05</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="H7" s="13">
         <v>4.1399999999999997</v>
       </c>
       <c r="I7" s="13">
-        <f t="shared" si="0"/>
-        <v>9.1199999999999992</v>
+        <f>(MAX(E7-0.2,0))^2+(MAX(F7-0.75,0))^2+(MAX(G7-4,0))^2 +(MAX(H7-4,0))^2</f>
+        <v>2.3199999999999863E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -709,29 +716,29 @@
         <v>3</v>
       </c>
       <c r="B8" s="11">
-        <v>3000</v>
+        <v>2600</v>
       </c>
       <c r="C8" s="11">
-        <v>10</v>
+        <v>8.6</v>
       </c>
       <c r="D8" s="11">
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
       <c r="E8" s="11">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F8" s="11">
-        <v>0.96</v>
+        <v>0.75</v>
       </c>
       <c r="G8" s="13">
-        <v>4</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="H8" s="13">
-        <v>4.16</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="I8" s="13">
-        <f t="shared" si="0"/>
-        <v>9.2800000000000011</v>
+        <f>(MAX(E8-0.2,0))^2+(MAX(F8-0.75,0))^2+(MAX(G8-4,0))^2 +(MAX(H8-4,0))^2</f>
+        <v>2.3199999999999863E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -739,29 +746,29 @@
         <v>3</v>
       </c>
       <c r="B9" s="11">
-        <v>3000</v>
+        <v>3100</v>
       </c>
       <c r="C9" s="11">
-        <v>10</v>
+        <v>8.6</v>
       </c>
       <c r="D9" s="11">
-        <v>0.11</v>
+        <v>0.16</v>
       </c>
       <c r="E9" s="11">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F9" s="11">
-        <v>1.04</v>
+        <v>0.74</v>
       </c>
       <c r="G9" s="13">
-        <v>3.97</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="H9" s="13">
-        <v>4.16</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="I9" s="13">
-        <f t="shared" si="0"/>
-        <v>9.32</v>
+        <f>(MAX(E9-0.2,0))^2+(MAX(F9-0.75,0))^2+(MAX(G9-4,0))^2 +(MAX(H9-4,0))^2</f>
+        <v>2.3199999999999863E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -772,26 +779,26 @@
         <v>3000</v>
       </c>
       <c r="C10" s="11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="11">
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
       <c r="E10" s="11">
         <v>0.15</v>
       </c>
       <c r="F10" s="11">
-        <v>1.1200000000000001</v>
+        <v>0.73</v>
       </c>
       <c r="G10" s="13">
-        <v>3.97</v>
+        <v>4.07</v>
       </c>
       <c r="H10" s="13">
-        <v>4.16</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="I10" s="13">
-        <f t="shared" si="0"/>
-        <v>9.4</v>
+        <f>(MAX(E10-0.2,0))^2+(MAX(F10-0.75,0))^2+(MAX(G10-4,0))^2 +(MAX(H10-4,0))^2</f>
+        <v>2.4499999999999949E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -805,23 +812,23 @@
         <v>10</v>
       </c>
       <c r="D11" s="11">
-        <v>0.09</v>
+        <v>0.16</v>
       </c>
       <c r="E11" s="11">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F11" s="11">
-        <v>1.23</v>
+        <v>0.74</v>
       </c>
       <c r="G11" s="13">
-        <v>3.92</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="H11" s="13">
-        <v>4.16</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="I11" s="13">
-        <f t="shared" si="0"/>
-        <v>9.4600000000000009</v>
+        <f>(MAX(E11-0.2,0))^2+(MAX(F11-0.75,0))^2+(MAX(G11-4,0))^2 +(MAX(H11-4,0))^2</f>
+        <v>2.6100000000000061E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -832,26 +839,26 @@
         <v>3000</v>
       </c>
       <c r="C12" s="11">
-        <v>10</v>
+        <v>8.9</v>
       </c>
       <c r="D12" s="11">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="E12" s="11">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F12" s="11">
-        <v>1.35</v>
+        <v>0.74</v>
       </c>
       <c r="G12" s="13">
-        <v>3.9</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="H12" s="13">
-        <v>4.17</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="I12" s="13">
-        <f t="shared" si="0"/>
-        <v>9.58</v>
+        <f>(MAX(E12-0.2,0))^2+(MAX(F12-0.75,0))^2+(MAX(G12-4,0))^2 +(MAX(H12-4,0))^2</f>
+        <v>2.6100000000000061E-2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -862,26 +869,26 @@
         <v>3000</v>
       </c>
       <c r="C13" s="11">
-        <v>10</v>
+        <v>8.6</v>
       </c>
       <c r="D13" s="11">
-        <v>7.0000000000000007E-2</v>
+        <v>0.16</v>
       </c>
       <c r="E13" s="11">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F13" s="11">
-        <v>1.51</v>
+        <v>0.74</v>
       </c>
       <c r="G13" s="13">
-        <v>3.84</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="H13" s="13">
-        <v>4.17</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="I13" s="13">
-        <f t="shared" si="0"/>
-        <v>9.68</v>
+        <f>(MAX(E13-0.2,0))^2+(MAX(F13-0.75,0))^2+(MAX(G13-4,0))^2 +(MAX(H13-4,0))^2</f>
+        <v>2.6100000000000061E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -892,26 +899,26 @@
         <v>3000</v>
       </c>
       <c r="C14" s="11">
-        <v>10</v>
+        <v>8.5</v>
       </c>
       <c r="D14" s="11">
-        <v>7.0000000000000007E-2</v>
+        <v>0.16</v>
       </c>
       <c r="E14" s="11">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F14" s="11">
-        <v>1.56</v>
+        <v>0.74</v>
       </c>
       <c r="G14" s="13">
-        <v>3.8</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="H14" s="13">
-        <v>4.18</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="I14" s="13">
-        <f t="shared" si="0"/>
-        <v>9.69</v>
+        <f>(MAX(E14-0.2,0))^2+(MAX(F14-0.75,0))^2+(MAX(G14-4,0))^2 +(MAX(H14-4,0))^2</f>
+        <v>2.6100000000000061E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -925,23 +932,23 @@
         <v>10</v>
       </c>
       <c r="D15" s="11">
-        <v>7.0000000000000007E-2</v>
+        <v>0.19</v>
       </c>
       <c r="E15" s="11">
         <v>0.15</v>
       </c>
       <c r="F15" s="11">
-        <v>1.61</v>
+        <v>0.63</v>
       </c>
       <c r="G15" s="13">
-        <v>3.78</v>
+        <v>4.07</v>
       </c>
       <c r="H15" s="13">
-        <v>4.18</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="I15" s="13">
-        <f t="shared" si="0"/>
-        <v>9.7199999999999989</v>
+        <f>(MAX(E15-0.2,0))^2+(MAX(F15-0.75,0))^2+(MAX(G15-4,0))^2 +(MAX(H15-4,0))^2</f>
+        <v>2.7400000000000146E-2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -949,29 +956,29 @@
         <v>3</v>
       </c>
       <c r="B16" s="11">
-        <v>3000</v>
+        <v>2700</v>
       </c>
       <c r="C16" s="11">
-        <v>10</v>
+        <v>8.6</v>
       </c>
       <c r="D16" s="11">
-        <v>0.06</v>
+        <v>0.16</v>
       </c>
       <c r="E16" s="11">
         <v>0.15</v>
       </c>
       <c r="F16" s="11">
-        <v>1.65</v>
+        <v>0.74</v>
       </c>
       <c r="G16" s="13">
-        <v>3.78</v>
+        <v>4.07</v>
       </c>
       <c r="H16" s="13">
-        <v>4.1900000000000004</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="I16" s="13">
-        <f t="shared" si="0"/>
-        <v>9.77</v>
+        <f>(MAX(E16-0.2,0))^2+(MAX(F16-0.75,0))^2+(MAX(G16-4,0))^2 +(MAX(H16-4,0))^2</f>
+        <v>2.7400000000000146E-2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -979,29 +986,29 @@
         <v>3</v>
       </c>
       <c r="B17" s="11">
-        <v>3000</v>
+        <v>2900</v>
       </c>
       <c r="C17" s="11">
-        <v>10</v>
+        <v>8.6</v>
       </c>
       <c r="D17" s="11">
-        <v>0.06</v>
+        <v>0.16</v>
       </c>
       <c r="E17" s="11">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F17" s="11">
-        <v>1.71</v>
+        <v>0.74</v>
       </c>
       <c r="G17" s="13">
-        <v>3.77</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="H17" s="13">
-        <v>4.1900000000000004</v>
+        <v>4.16</v>
       </c>
       <c r="I17" s="13">
-        <f t="shared" si="0"/>
-        <v>9.83</v>
+        <f>(MAX(E17-0.2,0))^2+(MAX(F17-0.75,0))^2+(MAX(G17-4,0))^2 +(MAX(H17-4,0))^2</f>
+        <v>2.92E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1009,10 +1016,10 @@
         <v>3</v>
       </c>
       <c r="B18" s="11">
-        <v>3000</v>
+        <v>2800</v>
       </c>
       <c r="C18" s="11">
-        <v>9</v>
+        <v>8.6</v>
       </c>
       <c r="D18" s="11">
         <v>0.16</v>
@@ -1021,17 +1028,17 @@
         <v>0.15</v>
       </c>
       <c r="F18" s="11">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
       <c r="G18" s="13">
         <v>4.07</v>
       </c>
       <c r="H18" s="13">
-        <v>4.1399999999999997</v>
+        <v>4.16</v>
       </c>
       <c r="I18" s="13">
-        <f t="shared" si="0"/>
-        <v>9.09</v>
+        <f>(MAX(E18-0.2,0))^2+(MAX(F18-0.75,0))^2+(MAX(G18-4,0))^2 +(MAX(H18-4,0))^2</f>
+        <v>3.0500000000000086E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1042,26 +1049,26 @@
         <v>3000</v>
       </c>
       <c r="C19" s="11">
-        <v>8.9</v>
+        <v>10</v>
       </c>
       <c r="D19" s="11">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="E19" s="11">
         <v>0.15</v>
       </c>
       <c r="F19" s="11">
-        <v>0.74</v>
+        <v>0.59</v>
       </c>
       <c r="G19" s="13">
-        <v>4.0599999999999996</v>
+        <v>4.08</v>
       </c>
       <c r="H19" s="13">
-        <v>4.1500000000000004</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="I19" s="13">
-        <f t="shared" si="0"/>
-        <v>9.1</v>
+        <f>(MAX(E19-0.2,0))^2+(MAX(F19-0.75,0))^2+(MAX(G19-4,0))^2 +(MAX(H19-4,0))^2</f>
+        <v>4.2500000000000156E-2</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1072,26 +1079,26 @@
         <v>3000</v>
       </c>
       <c r="C20" s="11">
-        <v>8.8000000000000007</v>
+        <v>10</v>
       </c>
       <c r="D20" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="E20" s="11">
         <v>0.16</v>
       </c>
-      <c r="E20" s="11">
-        <v>0.15</v>
-      </c>
       <c r="F20" s="11">
-        <v>0.74</v>
+        <v>0.52</v>
       </c>
       <c r="G20" s="13">
-        <v>4.05</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H20" s="13">
-        <v>4.1399999999999997</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="I20" s="13">
-        <f t="shared" si="0"/>
-        <v>9.0799999999999983</v>
+        <f>(MAX(E20-0.2,0))^2+(MAX(F20-0.75,0))^2+(MAX(G20-4,0))^2 +(MAX(H20-4,0))^2</f>
+        <v>6.2900000000000122E-2</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1102,26 +1109,26 @@
         <v>3000</v>
       </c>
       <c r="C21" s="11">
-        <v>8.6999999999999993</v>
+        <v>10</v>
       </c>
       <c r="D21" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="E21" s="11">
         <v>0.16</v>
       </c>
-      <c r="E21" s="11">
-        <v>0.15</v>
-      </c>
       <c r="F21" s="11">
-        <v>0.74</v>
+        <v>0.96</v>
       </c>
       <c r="G21" s="13">
-        <v>4.05</v>
+        <v>4</v>
       </c>
       <c r="H21" s="13">
-        <v>4.1399999999999997</v>
+        <v>4.16</v>
       </c>
       <c r="I21" s="13">
-        <f t="shared" si="0"/>
-        <v>9.0799999999999983</v>
+        <f>(MAX(E21-0.2,0))^2+(MAX(F21-0.75,0))^2+(MAX(G21-4,0))^2 +(MAX(H21-4,0))^2</f>
+        <v>6.970000000000004E-2</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1132,56 +1139,56 @@
         <v>3000</v>
       </c>
       <c r="C22" s="11">
-        <v>8.6</v>
+        <v>10</v>
       </c>
       <c r="D22" s="11">
-        <v>0.16</v>
+        <v>0.11</v>
       </c>
       <c r="E22" s="11">
         <v>0.15</v>
       </c>
       <c r="F22" s="11">
-        <v>0.74</v>
+        <v>1.04</v>
       </c>
       <c r="G22" s="13">
-        <v>4.0599999999999996</v>
+        <v>3.97</v>
       </c>
       <c r="H22" s="13">
-        <v>4.1500000000000004</v>
+        <v>4.16</v>
       </c>
       <c r="I22" s="13">
-        <f t="shared" si="0"/>
-        <v>9.1</v>
+        <f>(MAX(E22-0.2,0))^2+(MAX(F22-0.75,0))^2+(MAX(G22-4,0))^2 +(MAX(H22-4,0))^2</f>
+        <v>0.10970000000000008</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="11">
-        <v>3</v>
-      </c>
-      <c r="B23" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C23" s="11">
-        <v>8.5</v>
-      </c>
-      <c r="D23" s="11">
+      <c r="A23" s="15">
+        <v>3</v>
+      </c>
+      <c r="B23" s="15">
+        <v>3000</v>
+      </c>
+      <c r="C23" s="15">
+        <v>10</v>
+      </c>
+      <c r="D23" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="E23" s="15">
         <v>0.16</v>
       </c>
-      <c r="E23" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="F23" s="11">
-        <v>0.74</v>
-      </c>
-      <c r="G23" s="13">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="H23" s="13">
-        <v>4.1500000000000004</v>
+      <c r="F23" s="15">
+        <v>0.53</v>
+      </c>
+      <c r="G23" s="16">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H23" s="16">
+        <v>4.34</v>
       </c>
       <c r="I23" s="13">
-        <f t="shared" si="0"/>
-        <v>9.11</v>
+        <f>(MAX(E23-0.2,0))^2+(MAX(F23-0.75,0))^2+(MAX(G23-4,0))^2 +(MAX(H23-4,0))^2</f>
+        <v>0.12559999999999982</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1192,26 +1199,26 @@
         <v>3000</v>
       </c>
       <c r="C24" s="11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D24" s="11">
-        <v>0.16</v>
+        <v>0.3</v>
       </c>
       <c r="E24" s="11">
         <v>0.16</v>
       </c>
       <c r="F24" s="11">
-        <v>0.73</v>
+        <v>0.52</v>
       </c>
       <c r="G24" s="13">
-        <v>4.0599999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H24" s="13">
-        <v>4.1399999999999997</v>
+        <v>4.37</v>
       </c>
       <c r="I24" s="13">
-        <f t="shared" si="0"/>
-        <v>9.09</v>
+        <f>(MAX(E24-0.2,0))^2+(MAX(F24-0.75,0))^2+(MAX(G24-4,0))^2 +(MAX(H24-4,0))^2</f>
+        <v>0.1469</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1219,29 +1226,29 @@
         <v>3</v>
       </c>
       <c r="B25" s="11">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="C25" s="11">
-        <v>8.6</v>
+        <v>10</v>
       </c>
       <c r="D25" s="11">
-        <v>0.16</v>
+        <v>0.1</v>
       </c>
       <c r="E25" s="11">
         <v>0.15</v>
       </c>
       <c r="F25" s="11">
-        <v>0.73</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="G25" s="13">
-        <v>4.0599999999999996</v>
+        <v>3.97</v>
       </c>
       <c r="H25" s="13">
-        <v>4.13</v>
+        <v>4.16</v>
       </c>
       <c r="I25" s="13">
-        <f t="shared" si="0"/>
-        <v>9.07</v>
+        <f>(MAX(E25-0.2,0))^2+(MAX(F25-0.75,0))^2+(MAX(G25-4,0))^2 +(MAX(H25-4,0))^2</f>
+        <v>0.16250000000000012</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1249,29 +1256,29 @@
         <v>3</v>
       </c>
       <c r="B26" s="11">
-        <v>2600</v>
+        <v>3000</v>
       </c>
       <c r="C26" s="11">
-        <v>8.6</v>
+        <v>10</v>
       </c>
       <c r="D26" s="11">
-        <v>0.16</v>
+        <v>0.09</v>
       </c>
       <c r="E26" s="11">
         <v>0.15</v>
       </c>
       <c r="F26" s="11">
-        <v>0.75</v>
+        <v>1.23</v>
       </c>
       <c r="G26" s="13">
-        <v>4.0599999999999996</v>
+        <v>3.92</v>
       </c>
       <c r="H26" s="13">
-        <v>4.1399999999999997</v>
+        <v>4.16</v>
       </c>
       <c r="I26" s="13">
-        <f t="shared" si="0"/>
-        <v>9.1</v>
+        <f>(MAX(E26-0.2,0))^2+(MAX(F26-0.75,0))^2+(MAX(G26-4,0))^2 +(MAX(H26-4,0))^2</f>
+        <v>0.25600000000000006</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1279,29 +1286,29 @@
         <v>3</v>
       </c>
       <c r="B27" s="11">
-        <v>2700</v>
+        <v>3000</v>
       </c>
       <c r="C27" s="11">
-        <v>8.6</v>
+        <v>10</v>
       </c>
       <c r="D27" s="11">
+        <v>0.08</v>
+      </c>
+      <c r="E27" s="11">
         <v>0.16</v>
       </c>
-      <c r="E27" s="11">
-        <v>0.15</v>
-      </c>
       <c r="F27" s="11">
-        <v>0.74</v>
+        <v>1.35</v>
       </c>
       <c r="G27" s="13">
-        <v>4.07</v>
+        <v>3.9</v>
       </c>
       <c r="H27" s="13">
-        <v>4.1500000000000004</v>
+        <v>4.17</v>
       </c>
       <c r="I27" s="13">
-        <f t="shared" si="0"/>
-        <v>9.11</v>
+        <f>(MAX(E27-0.2,0))^2+(MAX(F27-0.75,0))^2+(MAX(G27-4,0))^2 +(MAX(H27-4,0))^2</f>
+        <v>0.38890000000000008</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1309,29 +1316,29 @@
         <v>3</v>
       </c>
       <c r="B28" s="11">
-        <v>2800</v>
+        <v>3000</v>
       </c>
       <c r="C28" s="11">
-        <v>8.6</v>
+        <v>10</v>
       </c>
       <c r="D28" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E28" s="11">
         <v>0.16</v>
       </c>
-      <c r="E28" s="11">
-        <v>0.15</v>
-      </c>
       <c r="F28" s="11">
-        <v>0.74</v>
+        <v>1.51</v>
       </c>
       <c r="G28" s="13">
-        <v>4.07</v>
+        <v>3.84</v>
       </c>
       <c r="H28" s="13">
-        <v>4.16</v>
+        <v>4.17</v>
       </c>
       <c r="I28" s="13">
-        <f t="shared" si="0"/>
-        <v>9.120000000000001</v>
+        <f>(MAX(E28-0.2,0))^2+(MAX(F28-0.75,0))^2+(MAX(G28-4,0))^2 +(MAX(H28-4,0))^2</f>
+        <v>0.60649999999999993</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1339,29 +1346,29 @@
         <v>3</v>
       </c>
       <c r="B29" s="11">
-        <v>2900</v>
+        <v>3000</v>
       </c>
       <c r="C29" s="11">
-        <v>8.6</v>
+        <v>10</v>
       </c>
       <c r="D29" s="11">
-        <v>0.16</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E29" s="11">
         <v>0.15</v>
       </c>
       <c r="F29" s="11">
-        <v>0.74</v>
+        <v>1.56</v>
       </c>
       <c r="G29" s="13">
-        <v>4.0599999999999996</v>
+        <v>3.8</v>
       </c>
       <c r="H29" s="13">
-        <v>4.16</v>
+        <v>4.18</v>
       </c>
       <c r="I29" s="13">
-        <f t="shared" si="0"/>
-        <v>9.11</v>
+        <f>(MAX(E29-0.2,0))^2+(MAX(F29-0.75,0))^2+(MAX(G29-4,0))^2 +(MAX(H29-4,0))^2</f>
+        <v>0.6885</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1372,26 +1379,26 @@
         <v>3000</v>
       </c>
       <c r="C30" s="11">
-        <v>8.6</v>
+        <v>10</v>
       </c>
       <c r="D30" s="11">
-        <v>0.16</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E30" s="11">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F30" s="11">
-        <v>0.74</v>
+        <v>1.61</v>
       </c>
       <c r="G30" s="13">
-        <v>4.0599999999999996</v>
+        <v>3.78</v>
       </c>
       <c r="H30" s="13">
-        <v>4.13</v>
+        <v>4.18</v>
       </c>
       <c r="I30" s="13">
-        <f t="shared" si="0"/>
-        <v>9.09</v>
+        <f>(MAX(E30-0.2,0))^2+(MAX(F30-0.75,0))^2+(MAX(G30-4,0))^2 +(MAX(H30-4,0))^2</f>
+        <v>0.77200000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1399,29 +1406,29 @@
         <v>3</v>
       </c>
       <c r="B31" s="11">
-        <v>3100</v>
+        <v>3000</v>
       </c>
       <c r="C31" s="11">
-        <v>8.6</v>
+        <v>10</v>
       </c>
       <c r="D31" s="11">
-        <v>0.16</v>
+        <v>0.06</v>
       </c>
       <c r="E31" s="11">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F31" s="11">
-        <v>0.74</v>
+        <v>1.65</v>
       </c>
       <c r="G31" s="13">
-        <v>4.0599999999999996</v>
+        <v>3.78</v>
       </c>
       <c r="H31" s="13">
-        <v>4.1399999999999997</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="I31" s="13">
-        <f t="shared" si="0"/>
-        <v>9.1</v>
+        <f>(MAX(E31-0.2,0))^2+(MAX(F31-0.75,0))^2+(MAX(G31-4,0))^2 +(MAX(H31-4,0))^2</f>
+        <v>0.84609999999999996</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1435,42 +1442,64 @@
         <v>10</v>
       </c>
       <c r="D32" s="12">
-        <v>0.3</v>
+        <v>0.06</v>
       </c>
       <c r="E32" s="12">
         <v>0.16</v>
       </c>
       <c r="F32" s="12">
-        <v>0.53</v>
+        <v>1.71</v>
       </c>
       <c r="G32" s="10">
-        <v>4.0999999999999996</v>
+        <v>3.77</v>
       </c>
       <c r="H32" s="10">
-        <v>4.34</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="I32" s="10">
-        <f t="shared" si="0"/>
-        <v>9.129999999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
+        <f>(MAX(E32-0.2,0))^2+(MAX(F32-0.75,0))^2+(MAX(G32-4,0))^2 +(MAX(H32-4,0))^2</f>
+        <v>0.95770000000000011</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I33" s="13"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I34" s="13"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I35" s="13"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I36" s="13"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I37" s="13"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I38" s="13"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I39" s="13"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>2999.6709384917081</v>
+      </c>
+      <c r="C40">
+        <v>9.1100693947327205</v>
+      </c>
+      <c r="D40">
+        <v>0.15038836079216389</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I33">
+    <sortCondition ref="I2:I33"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1479,7 +1508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I153"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScale="113" workbookViewId="0">
+    <sheetView zoomScale="113" workbookViewId="0">
       <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added plotting for ax and ay
</commit_message>
<xml_diff>
--- a/Engineering_Optimization/Sim3_Results.xlsx
+++ b/Engineering_Optimization/Sim3_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omarelsewify/Documents/GitHub/Past-Projects/Engineering_Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E7E0C9-CC39-A543-A5AD-134CD611CEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B3336B-56A8-DD4F-B56F-B771C8A4B6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="LARGE_SET" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$I$32</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -59,10 +62,10 @@
     <t>Max Longitudinal Acceleration</t>
   </si>
   <si>
-    <t>Sum</t>
+    <t>METRIC</t>
   </si>
   <si>
-    <t>METRIC</t>
+    <t>Sum</t>
   </si>
 </sst>
 </file>
@@ -171,14 +174,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -485,21 +488,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.6640625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.6640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -528,926 +531,926 @@
         <v>7</v>
       </c>
       <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="13">
+        <v>3</v>
+      </c>
+      <c r="B2" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C2" s="13">
+        <v>10</v>
+      </c>
+      <c r="D2" s="13">
+        <v>0.19</v>
+      </c>
+      <c r="E2" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0.63</v>
+      </c>
+      <c r="G2" s="14">
+        <v>4.07</v>
+      </c>
+      <c r="H2" s="14">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="I2" s="14">
+        <f>SUM(E2:H2)+10*(MAX(E2-0.2,0))^2+10*(MAX(F2-0.75,0))^2+(MAX(G2-4,0))^2 +(MAX(H2-4,0))^2</f>
+        <v>9.0274000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="13">
+        <v>3</v>
+      </c>
+      <c r="B3" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C3" s="13">
+        <v>10</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.59</v>
+      </c>
+      <c r="G3" s="14">
+        <v>4.08</v>
+      </c>
+      <c r="H3" s="14">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="I3" s="14">
+        <f>SUM(E3:H3)+10*(MAX(E3-0.2,0))^2+10*(MAX(F3-0.75,0))^2+(MAX(G3-4,0))^2 +(MAX(H3-4,0))^2</f>
+        <v>9.0525000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C4" s="13">
+        <v>10</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.52</v>
+      </c>
+      <c r="G4" s="14">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H4" s="14">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="I4" s="14">
+        <f>SUM(E4:H4)+10*(MAX(E4-0.2,0))^2+10*(MAX(F4-0.75,0))^2+(MAX(G4-4,0))^2 +(MAX(H4-4,0))^2</f>
+        <v>9.0729000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
+        <v>3</v>
+      </c>
+      <c r="B5" s="13">
+        <v>2500</v>
+      </c>
+      <c r="C5" s="13">
+        <v>8.6</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.73</v>
+      </c>
+      <c r="G5" s="14">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H5" s="14">
+        <v>4.13</v>
+      </c>
+      <c r="I5" s="14">
+        <f>SUM(E5:H5)+10*(MAX(E5-0.2,0))^2+10*(MAX(F5-0.75,0))^2+(MAX(G5-4,0))^2 +(MAX(H5-4,0))^2</f>
+        <v>9.0905000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="13">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C6" s="13">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.74</v>
+      </c>
+      <c r="G6" s="14">
+        <v>4.05</v>
+      </c>
+      <c r="H6" s="14">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I6" s="14">
+        <f>SUM(E6:H6)+10*(MAX(E6-0.2,0))^2+10*(MAX(F6-0.75,0))^2+(MAX(G6-4,0))^2 +(MAX(H6-4,0))^2</f>
+        <v>9.1020999999999983</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="13">
+        <v>3</v>
+      </c>
+      <c r="B7" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C7" s="13">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0.74</v>
+      </c>
+      <c r="G7" s="14">
+        <v>4.05</v>
+      </c>
+      <c r="H7" s="14">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I7" s="14">
+        <f>SUM(E7:H7)+10*(MAX(E7-0.2,0))^2+10*(MAX(F7-0.75,0))^2+(MAX(G7-4,0))^2 +(MAX(H7-4,0))^2</f>
+        <v>9.1020999999999983</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
+        <v>3</v>
+      </c>
+      <c r="B8" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C8" s="13">
+        <v>8.6</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0.74</v>
+      </c>
+      <c r="G8" s="14">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H8" s="14">
+        <v>4.13</v>
+      </c>
+      <c r="I8" s="14">
+        <f>SUM(E8:H8)+10*(MAX(E8-0.2,0))^2+10*(MAX(F8-0.75,0))^2+(MAX(G8-4,0))^2 +(MAX(H8-4,0))^2</f>
+        <v>9.1105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="13">
+        <v>3</v>
+      </c>
+      <c r="B9" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C9" s="13">
+        <v>8</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="F9" s="13">
+        <v>0.73</v>
+      </c>
+      <c r="G9" s="14">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H9" s="14">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I9" s="14">
+        <f>SUM(E9:H9)+10*(MAX(E9-0.2,0))^2+10*(MAX(F9-0.75,0))^2+(MAX(G9-4,0))^2 +(MAX(H9-4,0))^2</f>
+        <v>9.1132000000000009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="13">
+        <v>3</v>
+      </c>
+      <c r="B10" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C10" s="13">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="11">
-        <v>3</v>
-      </c>
-      <c r="B2" s="11">
-        <v>2500</v>
-      </c>
-      <c r="C2" s="11">
+      <c r="D10" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0.73</v>
+      </c>
+      <c r="G10" s="14">
+        <v>4.07</v>
+      </c>
+      <c r="H10" s="14">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I10" s="14">
+        <f>SUM(E10:H10)+10*(MAX(E10-0.2,0))^2+10*(MAX(F10-0.75,0))^2+(MAX(G10-4,0))^2 +(MAX(H10-4,0))^2</f>
+        <v>9.1144999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="13">
+        <v>3</v>
+      </c>
+      <c r="B11" s="13">
+        <v>2600</v>
+      </c>
+      <c r="C11" s="13">
         <v>8.6</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D11" s="13">
         <v>0.16</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E11" s="13">
         <v>0.15</v>
       </c>
-      <c r="F2" s="11">
-        <v>0.73</v>
-      </c>
-      <c r="G2" s="13">
+      <c r="F11" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="G11" s="14">
         <v>4.0599999999999996</v>
       </c>
-      <c r="H2" s="13">
-        <v>4.13</v>
-      </c>
-      <c r="I2" s="13">
-        <f>(MAX(E2-0.2,0))^2+(MAX(F2-0.75,0))^2+(MAX(G2-4,0))^2 +(MAX(H2-4,0))^2</f>
-        <v>2.0499999999999925E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="15">
-        <v>3</v>
-      </c>
-      <c r="B3" s="15">
-        <v>3000</v>
-      </c>
-      <c r="C3" s="15">
+      <c r="H11" s="14">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I11" s="14">
+        <f>SUM(E11:H11)+10*(MAX(E11-0.2,0))^2+10*(MAX(F11-0.75,0))^2+(MAX(G11-4,0))^2 +(MAX(H11-4,0))^2</f>
+        <v>9.1232000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="13">
+        <v>3</v>
+      </c>
+      <c r="B12" s="13">
+        <v>3100</v>
+      </c>
+      <c r="C12" s="13">
         <v>8.6</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D12" s="13">
         <v>0.16</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E12" s="13">
         <v>0.16</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F12" s="13">
         <v>0.74</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G12" s="14">
         <v>4.0599999999999996</v>
       </c>
-      <c r="H3" s="16">
-        <v>4.13</v>
-      </c>
-      <c r="I3" s="13">
-        <f>(MAX(E3-0.2,0))^2+(MAX(F3-0.75,0))^2+(MAX(G3-4,0))^2 +(MAX(H3-4,0))^2</f>
-        <v>2.0499999999999925E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="11">
-        <v>3</v>
-      </c>
-      <c r="B4" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C4" s="11">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="D4" s="11">
+      <c r="H12" s="14">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I12" s="14">
+        <f>SUM(E12:H12)+10*(MAX(E12-0.2,0))^2+10*(MAX(F12-0.75,0))^2+(MAX(G12-4,0))^2 +(MAX(H12-4,0))^2</f>
+        <v>9.1232000000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="13">
+        <v>3</v>
+      </c>
+      <c r="B13" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C13" s="13">
+        <v>8.9</v>
+      </c>
+      <c r="D13" s="13">
         <v>0.16</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E13" s="13">
         <v>0.15</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F13" s="13">
         <v>0.74</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G13" s="14">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H13" s="14">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="I13" s="14">
+        <f>SUM(E13:H13)+10*(MAX(E13-0.2,0))^2+10*(MAX(F13-0.75,0))^2+(MAX(G13-4,0))^2 +(MAX(H13-4,0))^2</f>
+        <v>9.126100000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="13">
+        <v>3</v>
+      </c>
+      <c r="B14" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C14" s="13">
+        <v>8.6</v>
+      </c>
+      <c r="D14" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0.74</v>
+      </c>
+      <c r="G14" s="14">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H14" s="14">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="I14" s="14">
+        <f>SUM(E14:H14)+10*(MAX(E14-0.2,0))^2+10*(MAX(F14-0.75,0))^2+(MAX(G14-4,0))^2 +(MAX(H14-4,0))^2</f>
+        <v>9.126100000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="13">
+        <v>3</v>
+      </c>
+      <c r="B15" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C15" s="13">
+        <v>10</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="F15" s="13">
+        <v>0.74</v>
+      </c>
+      <c r="G15" s="14">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H15" s="14">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="I15" s="14">
+        <f>SUM(E15:H15)+10*(MAX(E15-0.2,0))^2+10*(MAX(F15-0.75,0))^2+(MAX(G15-4,0))^2 +(MAX(H15-4,0))^2</f>
+        <v>9.1361000000000008</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="13">
+        <v>3</v>
+      </c>
+      <c r="B16" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C16" s="13">
+        <v>8.5</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="E16" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="F16" s="13">
+        <v>0.74</v>
+      </c>
+      <c r="G16" s="14">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H16" s="14">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="I16" s="14">
+        <f>SUM(E16:H16)+10*(MAX(E16-0.2,0))^2+10*(MAX(F16-0.75,0))^2+(MAX(G16-4,0))^2 +(MAX(H16-4,0))^2</f>
+        <v>9.1361000000000008</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="13">
+        <v>3</v>
+      </c>
+      <c r="B17" s="13">
+        <v>2700</v>
+      </c>
+      <c r="C17" s="13">
+        <v>8.6</v>
+      </c>
+      <c r="D17" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="E17" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F17" s="13">
+        <v>0.74</v>
+      </c>
+      <c r="G17" s="14">
+        <v>4.07</v>
+      </c>
+      <c r="H17" s="14">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="I17" s="14">
+        <f>SUM(E17:H17)+10*(MAX(E17-0.2,0))^2+10*(MAX(F17-0.75,0))^2+(MAX(G17-4,0))^2 +(MAX(H17-4,0))^2</f>
+        <v>9.1373999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="13">
+        <v>3</v>
+      </c>
+      <c r="B18" s="13">
+        <v>2900</v>
+      </c>
+      <c r="C18" s="13">
+        <v>8.6</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="E18" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F18" s="13">
+        <v>0.74</v>
+      </c>
+      <c r="G18" s="14">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H18" s="14">
+        <v>4.16</v>
+      </c>
+      <c r="I18" s="14">
+        <f>SUM(E18:H18)+10*(MAX(E18-0.2,0))^2+10*(MAX(F18-0.75,0))^2+(MAX(G18-4,0))^2 +(MAX(H18-4,0))^2</f>
+        <v>9.1392000000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="13">
+        <v>3</v>
+      </c>
+      <c r="B19" s="13">
+        <v>2800</v>
+      </c>
+      <c r="C19" s="13">
+        <v>8.6</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="E19" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F19" s="13">
+        <v>0.74</v>
+      </c>
+      <c r="G19" s="14">
+        <v>4.07</v>
+      </c>
+      <c r="H19" s="14">
+        <v>4.16</v>
+      </c>
+      <c r="I19" s="14">
+        <f>SUM(E19:H19)+10*(MAX(E19-0.2,0))^2+10*(MAX(F19-0.75,0))^2+(MAX(G19-4,0))^2 +(MAX(H19-4,0))^2</f>
+        <v>9.150500000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="13">
+        <v>3</v>
+      </c>
+      <c r="B20" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C20" s="13">
+        <v>10</v>
+      </c>
+      <c r="D20" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F20" s="13">
+        <v>0.78</v>
+      </c>
+      <c r="G20" s="14">
         <v>4.05</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H20" s="14">
         <v>4.1399999999999997</v>
       </c>
-      <c r="I4" s="13">
-        <f>(MAX(E4-0.2,0))^2+(MAX(F4-0.75,0))^2+(MAX(G4-4,0))^2 +(MAX(H4-4,0))^2</f>
-        <v>2.2099999999999891E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="11">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C5" s="11">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="D5" s="11">
+      <c r="I20" s="14">
+        <f>SUM(E20:H20)+10*(MAX(E20-0.2,0))^2+10*(MAX(F20-0.75,0))^2+(MAX(G20-4,0))^2 +(MAX(H20-4,0))^2</f>
+        <v>9.1510999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="13">
+        <v>3</v>
+      </c>
+      <c r="B21" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C21" s="13">
+        <v>10</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="E21" s="13">
         <v>0.16</v>
       </c>
-      <c r="E5" s="11">
+      <c r="F21" s="13">
+        <v>0.53</v>
+      </c>
+      <c r="G21" s="14">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H21" s="14">
+        <v>4.34</v>
+      </c>
+      <c r="I21" s="14">
+        <f>SUM(E21:H21)+10*(MAX(E21-0.2,0))^2+10*(MAX(F21-0.75,0))^2+(MAX(G21-4,0))^2 +(MAX(H21-4,0))^2</f>
+        <v>9.2555999999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="13">
+        <v>3</v>
+      </c>
+      <c r="B22" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C22" s="13">
+        <v>10</v>
+      </c>
+      <c r="D22" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="E22" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="F22" s="13">
+        <v>0.52</v>
+      </c>
+      <c r="G22" s="14">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H22" s="14">
+        <v>4.37</v>
+      </c>
+      <c r="I22" s="14">
+        <f>SUM(E22:H22)+10*(MAX(E22-0.2,0))^2+10*(MAX(F22-0.75,0))^2+(MAX(G22-4,0))^2 +(MAX(H22-4,0))^2</f>
+        <v>9.2968999999999991</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="13">
+        <v>3</v>
+      </c>
+      <c r="B23" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C23" s="13">
+        <v>10</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0.12</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.16</v>
+      </c>
+      <c r="F23" s="13">
+        <v>0.96</v>
+      </c>
+      <c r="G23" s="14">
+        <v>4</v>
+      </c>
+      <c r="H23" s="14">
+        <v>4.16</v>
+      </c>
+      <c r="I23" s="14">
+        <f>SUM(E23:H23)+10*(MAX(E23-0.2,0))^2+10*(MAX(F23-0.75,0))^2+(MAX(G23-4,0))^2 +(MAX(H23-4,0))^2</f>
+        <v>9.7466000000000008</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="13">
+        <v>3</v>
+      </c>
+      <c r="B24" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C24" s="13">
+        <v>10</v>
+      </c>
+      <c r="D24" s="13">
+        <v>0.11</v>
+      </c>
+      <c r="E24" s="13">
         <v>0.15</v>
       </c>
-      <c r="F5" s="11">
-        <v>0.74</v>
-      </c>
-      <c r="G5" s="13">
-        <v>4.05</v>
-      </c>
-      <c r="H5" s="13">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="I5" s="13">
-        <f>(MAX(E5-0.2,0))^2+(MAX(F5-0.75,0))^2+(MAX(G5-4,0))^2 +(MAX(H5-4,0))^2</f>
-        <v>2.2099999999999891E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="11">
-        <v>3</v>
-      </c>
-      <c r="B6" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C6" s="11">
+      <c r="F24" s="13">
+        <v>1.04</v>
+      </c>
+      <c r="G24" s="14">
+        <v>3.97</v>
+      </c>
+      <c r="H24" s="14">
+        <v>4.16</v>
+      </c>
+      <c r="I24" s="14">
+        <f>SUM(E24:H24)+10*(MAX(E24-0.2,0))^2+10*(MAX(F24-0.75,0))^2+(MAX(G24-4,0))^2 +(MAX(H24-4,0))^2</f>
+        <v>10.186600000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="13">
+        <v>3</v>
+      </c>
+      <c r="B25" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C25" s="13">
         <v>10</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D25" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E25" s="13">
         <v>0.15</v>
       </c>
-      <c r="E6" s="11">
+      <c r="F25" s="13">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G25" s="14">
+        <v>3.97</v>
+      </c>
+      <c r="H25" s="14">
+        <v>4.16</v>
+      </c>
+      <c r="I25" s="14">
+        <f>SUM(E25:H25)+10*(MAX(E25-0.2,0))^2+10*(MAX(F25-0.75,0))^2+(MAX(G25-4,0))^2 +(MAX(H25-4,0))^2</f>
+        <v>10.794600000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="13">
+        <v>3</v>
+      </c>
+      <c r="B26" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C26" s="13">
+        <v>10</v>
+      </c>
+      <c r="D26" s="13">
+        <v>0.09</v>
+      </c>
+      <c r="E26" s="13">
         <v>0.15</v>
       </c>
-      <c r="F6" s="11">
-        <v>0.78</v>
-      </c>
-      <c r="G6" s="13">
-        <v>4.05</v>
-      </c>
-      <c r="H6" s="13">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="I6" s="13">
-        <f>(MAX(E6-0.2,0))^2+(MAX(F6-0.75,0))^2+(MAX(G6-4,0))^2 +(MAX(H6-4,0))^2</f>
-        <v>2.2999999999999892E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="11">
-        <v>3</v>
-      </c>
-      <c r="B7" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C7" s="11">
-        <v>8</v>
-      </c>
-      <c r="D7" s="11">
+      <c r="F26" s="13">
+        <v>1.23</v>
+      </c>
+      <c r="G26" s="14">
+        <v>3.92</v>
+      </c>
+      <c r="H26" s="14">
+        <v>4.16</v>
+      </c>
+      <c r="I26" s="14">
+        <f>SUM(E26:H26)+10*(MAX(E26-0.2,0))^2+10*(MAX(F26-0.75,0))^2+(MAX(G26-4,0))^2 +(MAX(H26-4,0))^2</f>
+        <v>11.789600000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="13">
+        <v>3</v>
+      </c>
+      <c r="B27" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C27" s="13">
+        <v>10</v>
+      </c>
+      <c r="D27" s="13">
+        <v>0.08</v>
+      </c>
+      <c r="E27" s="13">
         <v>0.16</v>
       </c>
-      <c r="E7" s="11">
+      <c r="F27" s="13">
+        <v>1.35</v>
+      </c>
+      <c r="G27" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="H27" s="14">
+        <v>4.17</v>
+      </c>
+      <c r="I27" s="14">
+        <f>SUM(E27:H27)+10*(MAX(E27-0.2,0))^2+10*(MAX(F27-0.75,0))^2+(MAX(G27-4,0))^2 +(MAX(H27-4,0))^2</f>
+        <v>13.208900000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="13">
+        <v>3</v>
+      </c>
+      <c r="B28" s="13">
+        <v>3000</v>
+      </c>
+      <c r="C28" s="13">
+        <v>10</v>
+      </c>
+      <c r="D28" s="13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E28" s="13">
         <v>0.16</v>
       </c>
-      <c r="F7" s="11">
-        <v>0.73</v>
-      </c>
-      <c r="G7" s="13">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="H7" s="13">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="I7" s="13">
-        <f>(MAX(E7-0.2,0))^2+(MAX(F7-0.75,0))^2+(MAX(G7-4,0))^2 +(MAX(H7-4,0))^2</f>
-        <v>2.3199999999999863E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="11">
-        <v>3</v>
-      </c>
-      <c r="B8" s="11">
-        <v>2600</v>
-      </c>
-      <c r="C8" s="11">
-        <v>8.6</v>
-      </c>
-      <c r="D8" s="11">
+      <c r="F28" s="13">
+        <v>1.51</v>
+      </c>
+      <c r="G28" s="14">
+        <v>3.84</v>
+      </c>
+      <c r="H28" s="14">
+        <v>4.17</v>
+      </c>
+      <c r="I28" s="14">
+        <f>SUM(E28:H28)+10*(MAX(E28-0.2,0))^2+10*(MAX(F28-0.75,0))^2+(MAX(G28-4,0))^2 +(MAX(H28-4,0))^2</f>
+        <v>15.4849</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="15">
+        <v>3</v>
+      </c>
+      <c r="B29" s="15">
+        <v>3000</v>
+      </c>
+      <c r="C29" s="15">
+        <v>10</v>
+      </c>
+      <c r="D29" s="15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E29" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="F29" s="15">
+        <v>1.56</v>
+      </c>
+      <c r="G29" s="16">
+        <v>3.8</v>
+      </c>
+      <c r="H29" s="16">
+        <v>4.18</v>
+      </c>
+      <c r="I29" s="14">
+        <f>SUM(E29:H29)+10*(MAX(E29-0.2,0))^2+10*(MAX(F29-0.75,0))^2+(MAX(G29-4,0))^2 +(MAX(H29-4,0))^2</f>
+        <v>16.2834</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="15">
+        <v>3</v>
+      </c>
+      <c r="B30" s="15">
+        <v>3000</v>
+      </c>
+      <c r="C30" s="15">
+        <v>10</v>
+      </c>
+      <c r="D30" s="15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E30" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="F30" s="15">
+        <v>1.61</v>
+      </c>
+      <c r="G30" s="16">
+        <v>3.78</v>
+      </c>
+      <c r="H30" s="16">
+        <v>4.18</v>
+      </c>
+      <c r="I30" s="14">
+        <f>SUM(E30:H30)+10*(MAX(E30-0.2,0))^2+10*(MAX(F30-0.75,0))^2+(MAX(G30-4,0))^2 +(MAX(H30-4,0))^2</f>
+        <v>17.148399999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="15">
+        <v>3</v>
+      </c>
+      <c r="B31" s="15">
+        <v>3000</v>
+      </c>
+      <c r="C31" s="15">
+        <v>10</v>
+      </c>
+      <c r="D31" s="15">
+        <v>0.06</v>
+      </c>
+      <c r="E31" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="F31" s="15">
+        <v>1.65</v>
+      </c>
+      <c r="G31" s="16">
+        <v>3.78</v>
+      </c>
+      <c r="H31" s="16">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="I31" s="14">
+        <f>SUM(E31:H31)+10*(MAX(E31-0.2,0))^2+10*(MAX(F31-0.75,0))^2+(MAX(G31-4,0))^2 +(MAX(H31-4,0))^2</f>
+        <v>17.906099999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="11">
+        <v>3</v>
+      </c>
+      <c r="B32" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C32" s="11">
+        <v>10</v>
+      </c>
+      <c r="D32" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="E32" s="11">
         <v>0.16</v>
       </c>
-      <c r="E8" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F8" s="11">
-        <v>0.75</v>
-      </c>
-      <c r="G8" s="13">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="H8" s="13">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="I8" s="13">
-        <f>(MAX(E8-0.2,0))^2+(MAX(F8-0.75,0))^2+(MAX(G8-4,0))^2 +(MAX(H8-4,0))^2</f>
-        <v>2.3199999999999863E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="11">
-        <v>3</v>
-      </c>
-      <c r="B9" s="11">
-        <v>3100</v>
-      </c>
-      <c r="C9" s="11">
-        <v>8.6</v>
-      </c>
-      <c r="D9" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="E9" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="F9" s="11">
-        <v>0.74</v>
-      </c>
-      <c r="G9" s="13">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="H9" s="13">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="I9" s="13">
-        <f>(MAX(E9-0.2,0))^2+(MAX(F9-0.75,0))^2+(MAX(G9-4,0))^2 +(MAX(H9-4,0))^2</f>
-        <v>2.3199999999999863E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="11">
-        <v>3</v>
-      </c>
-      <c r="B10" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C10" s="11">
-        <v>9</v>
-      </c>
-      <c r="D10" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="E10" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F10" s="11">
-        <v>0.73</v>
-      </c>
-      <c r="G10" s="13">
-        <v>4.07</v>
-      </c>
-      <c r="H10" s="13">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="I10" s="13">
-        <f>(MAX(E10-0.2,0))^2+(MAX(F10-0.75,0))^2+(MAX(G10-4,0))^2 +(MAX(H10-4,0))^2</f>
-        <v>2.4499999999999949E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="11">
-        <v>3</v>
-      </c>
-      <c r="B11" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C11" s="11">
-        <v>10</v>
-      </c>
-      <c r="D11" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="E11" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="F11" s="11">
-        <v>0.74</v>
-      </c>
-      <c r="G11" s="13">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="H11" s="13">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="I11" s="13">
-        <f>(MAX(E11-0.2,0))^2+(MAX(F11-0.75,0))^2+(MAX(G11-4,0))^2 +(MAX(H11-4,0))^2</f>
-        <v>2.6100000000000061E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="11">
-        <v>3</v>
-      </c>
-      <c r="B12" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C12" s="11">
-        <v>8.9</v>
-      </c>
-      <c r="D12" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="E12" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F12" s="11">
-        <v>0.74</v>
-      </c>
-      <c r="G12" s="13">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="H12" s="13">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="I12" s="13">
-        <f>(MAX(E12-0.2,0))^2+(MAX(F12-0.75,0))^2+(MAX(G12-4,0))^2 +(MAX(H12-4,0))^2</f>
-        <v>2.6100000000000061E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="11">
-        <v>3</v>
-      </c>
-      <c r="B13" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C13" s="11">
-        <v>8.6</v>
-      </c>
-      <c r="D13" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="E13" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F13" s="11">
-        <v>0.74</v>
-      </c>
-      <c r="G13" s="13">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="H13" s="13">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="I13" s="13">
-        <f>(MAX(E13-0.2,0))^2+(MAX(F13-0.75,0))^2+(MAX(G13-4,0))^2 +(MAX(H13-4,0))^2</f>
-        <v>2.6100000000000061E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="11">
-        <v>3</v>
-      </c>
-      <c r="B14" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C14" s="11">
-        <v>8.5</v>
-      </c>
-      <c r="D14" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="E14" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="F14" s="11">
-        <v>0.74</v>
-      </c>
-      <c r="G14" s="13">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="H14" s="13">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="I14" s="13">
-        <f>(MAX(E14-0.2,0))^2+(MAX(F14-0.75,0))^2+(MAX(G14-4,0))^2 +(MAX(H14-4,0))^2</f>
-        <v>2.6100000000000061E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="11">
-        <v>3</v>
-      </c>
-      <c r="B15" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C15" s="11">
-        <v>10</v>
-      </c>
-      <c r="D15" s="11">
-        <v>0.19</v>
-      </c>
-      <c r="E15" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F15" s="11">
-        <v>0.63</v>
-      </c>
-      <c r="G15" s="13">
-        <v>4.07</v>
-      </c>
-      <c r="H15" s="13">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="I15" s="13">
-        <f>(MAX(E15-0.2,0))^2+(MAX(F15-0.75,0))^2+(MAX(G15-4,0))^2 +(MAX(H15-4,0))^2</f>
-        <v>2.7400000000000146E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="11">
-        <v>3</v>
-      </c>
-      <c r="B16" s="11">
-        <v>2700</v>
-      </c>
-      <c r="C16" s="11">
-        <v>8.6</v>
-      </c>
-      <c r="D16" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="E16" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F16" s="11">
-        <v>0.74</v>
-      </c>
-      <c r="G16" s="13">
-        <v>4.07</v>
-      </c>
-      <c r="H16" s="13">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="I16" s="13">
-        <f>(MAX(E16-0.2,0))^2+(MAX(F16-0.75,0))^2+(MAX(G16-4,0))^2 +(MAX(H16-4,0))^2</f>
-        <v>2.7400000000000146E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="11">
-        <v>3</v>
-      </c>
-      <c r="B17" s="11">
-        <v>2900</v>
-      </c>
-      <c r="C17" s="11">
-        <v>8.6</v>
-      </c>
-      <c r="D17" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="E17" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F17" s="11">
-        <v>0.74</v>
-      </c>
-      <c r="G17" s="13">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="H17" s="13">
-        <v>4.16</v>
-      </c>
-      <c r="I17" s="13">
-        <f>(MAX(E17-0.2,0))^2+(MAX(F17-0.75,0))^2+(MAX(G17-4,0))^2 +(MAX(H17-4,0))^2</f>
-        <v>2.92E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="11">
-        <v>3</v>
-      </c>
-      <c r="B18" s="11">
-        <v>2800</v>
-      </c>
-      <c r="C18" s="11">
-        <v>8.6</v>
-      </c>
-      <c r="D18" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="E18" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F18" s="11">
-        <v>0.74</v>
-      </c>
-      <c r="G18" s="13">
-        <v>4.07</v>
-      </c>
-      <c r="H18" s="13">
-        <v>4.16</v>
-      </c>
-      <c r="I18" s="13">
-        <f>(MAX(E18-0.2,0))^2+(MAX(F18-0.75,0))^2+(MAX(G18-4,0))^2 +(MAX(H18-4,0))^2</f>
-        <v>3.0500000000000086E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="11">
-        <v>3</v>
-      </c>
-      <c r="B19" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C19" s="11">
-        <v>10</v>
-      </c>
-      <c r="D19" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E19" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F19" s="11">
-        <v>0.59</v>
-      </c>
-      <c r="G19" s="13">
-        <v>4.08</v>
-      </c>
-      <c r="H19" s="13">
-        <v>4.1900000000000004</v>
-      </c>
-      <c r="I19" s="13">
-        <f>(MAX(E19-0.2,0))^2+(MAX(F19-0.75,0))^2+(MAX(G19-4,0))^2 +(MAX(H19-4,0))^2</f>
-        <v>4.2500000000000156E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="11">
-        <v>3</v>
-      </c>
-      <c r="B20" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C20" s="11">
-        <v>10</v>
-      </c>
-      <c r="D20" s="11">
-        <v>0.25</v>
-      </c>
-      <c r="E20" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="F20" s="11">
-        <v>0.52</v>
-      </c>
-      <c r="G20" s="13">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="H20" s="13">
-        <v>4.2300000000000004</v>
-      </c>
-      <c r="I20" s="13">
-        <f>(MAX(E20-0.2,0))^2+(MAX(F20-0.75,0))^2+(MAX(G20-4,0))^2 +(MAX(H20-4,0))^2</f>
-        <v>6.2900000000000122E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="11">
-        <v>3</v>
-      </c>
-      <c r="B21" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C21" s="11">
-        <v>10</v>
-      </c>
-      <c r="D21" s="11">
-        <v>0.12</v>
-      </c>
-      <c r="E21" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="F21" s="11">
-        <v>0.96</v>
-      </c>
-      <c r="G21" s="13">
-        <v>4</v>
-      </c>
-      <c r="H21" s="13">
-        <v>4.16</v>
-      </c>
-      <c r="I21" s="13">
-        <f>(MAX(E21-0.2,0))^2+(MAX(F21-0.75,0))^2+(MAX(G21-4,0))^2 +(MAX(H21-4,0))^2</f>
-        <v>6.970000000000004E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="11">
-        <v>3</v>
-      </c>
-      <c r="B22" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C22" s="11">
-        <v>10</v>
-      </c>
-      <c r="D22" s="11">
-        <v>0.11</v>
-      </c>
-      <c r="E22" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F22" s="11">
-        <v>1.04</v>
-      </c>
-      <c r="G22" s="13">
-        <v>3.97</v>
-      </c>
-      <c r="H22" s="13">
-        <v>4.16</v>
-      </c>
-      <c r="I22" s="13">
-        <f>(MAX(E22-0.2,0))^2+(MAX(F22-0.75,0))^2+(MAX(G22-4,0))^2 +(MAX(H22-4,0))^2</f>
-        <v>0.10970000000000008</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="15">
-        <v>3</v>
-      </c>
-      <c r="B23" s="15">
-        <v>3000</v>
-      </c>
-      <c r="C23" s="15">
-        <v>10</v>
-      </c>
-      <c r="D23" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="E23" s="15">
-        <v>0.16</v>
-      </c>
-      <c r="F23" s="15">
-        <v>0.53</v>
-      </c>
-      <c r="G23" s="16">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="H23" s="16">
-        <v>4.34</v>
-      </c>
-      <c r="I23" s="13">
-        <f>(MAX(E23-0.2,0))^2+(MAX(F23-0.75,0))^2+(MAX(G23-4,0))^2 +(MAX(H23-4,0))^2</f>
-        <v>0.12559999999999982</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="11">
-        <v>3</v>
-      </c>
-      <c r="B24" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C24" s="11">
-        <v>10</v>
-      </c>
-      <c r="D24" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="E24" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="F24" s="11">
-        <v>0.52</v>
-      </c>
-      <c r="G24" s="13">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="H24" s="13">
-        <v>4.37</v>
-      </c>
-      <c r="I24" s="13">
-        <f>(MAX(E24-0.2,0))^2+(MAX(F24-0.75,0))^2+(MAX(G24-4,0))^2 +(MAX(H24-4,0))^2</f>
-        <v>0.1469</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="11">
-        <v>3</v>
-      </c>
-      <c r="B25" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C25" s="11">
-        <v>10</v>
-      </c>
-      <c r="D25" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="E25" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F25" s="11">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="G25" s="13">
-        <v>3.97</v>
-      </c>
-      <c r="H25" s="13">
-        <v>4.16</v>
-      </c>
-      <c r="I25" s="13">
-        <f>(MAX(E25-0.2,0))^2+(MAX(F25-0.75,0))^2+(MAX(G25-4,0))^2 +(MAX(H25-4,0))^2</f>
-        <v>0.16250000000000012</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="11">
-        <v>3</v>
-      </c>
-      <c r="B26" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C26" s="11">
-        <v>10</v>
-      </c>
-      <c r="D26" s="11">
-        <v>0.09</v>
-      </c>
-      <c r="E26" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F26" s="11">
-        <v>1.23</v>
-      </c>
-      <c r="G26" s="13">
-        <v>3.92</v>
-      </c>
-      <c r="H26" s="13">
-        <v>4.16</v>
-      </c>
-      <c r="I26" s="13">
-        <f>(MAX(E26-0.2,0))^2+(MAX(F26-0.75,0))^2+(MAX(G26-4,0))^2 +(MAX(H26-4,0))^2</f>
-        <v>0.25600000000000006</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="11">
-        <v>3</v>
-      </c>
-      <c r="B27" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C27" s="11">
-        <v>10</v>
-      </c>
-      <c r="D27" s="11">
-        <v>0.08</v>
-      </c>
-      <c r="E27" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="F27" s="11">
-        <v>1.35</v>
-      </c>
-      <c r="G27" s="13">
-        <v>3.9</v>
-      </c>
-      <c r="H27" s="13">
-        <v>4.17</v>
-      </c>
-      <c r="I27" s="13">
-        <f>(MAX(E27-0.2,0))^2+(MAX(F27-0.75,0))^2+(MAX(G27-4,0))^2 +(MAX(H27-4,0))^2</f>
-        <v>0.38890000000000008</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="11">
-        <v>3</v>
-      </c>
-      <c r="B28" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C28" s="11">
-        <v>10</v>
-      </c>
-      <c r="D28" s="11">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E28" s="11">
-        <v>0.16</v>
-      </c>
-      <c r="F28" s="11">
-        <v>1.51</v>
-      </c>
-      <c r="G28" s="13">
-        <v>3.84</v>
-      </c>
-      <c r="H28" s="13">
-        <v>4.17</v>
-      </c>
-      <c r="I28" s="13">
-        <f>(MAX(E28-0.2,0))^2+(MAX(F28-0.75,0))^2+(MAX(G28-4,0))^2 +(MAX(H28-4,0))^2</f>
-        <v>0.60649999999999993</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="11">
-        <v>3</v>
-      </c>
-      <c r="B29" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C29" s="11">
-        <v>10</v>
-      </c>
-      <c r="D29" s="11">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E29" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F29" s="11">
-        <v>1.56</v>
-      </c>
-      <c r="G29" s="13">
-        <v>3.8</v>
-      </c>
-      <c r="H29" s="13">
-        <v>4.18</v>
-      </c>
-      <c r="I29" s="13">
-        <f>(MAX(E29-0.2,0))^2+(MAX(F29-0.75,0))^2+(MAX(G29-4,0))^2 +(MAX(H29-4,0))^2</f>
-        <v>0.6885</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="11">
-        <v>3</v>
-      </c>
-      <c r="B30" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C30" s="11">
-        <v>10</v>
-      </c>
-      <c r="D30" s="11">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E30" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F30" s="11">
-        <v>1.61</v>
-      </c>
-      <c r="G30" s="13">
-        <v>3.78</v>
-      </c>
-      <c r="H30" s="13">
-        <v>4.18</v>
-      </c>
-      <c r="I30" s="13">
-        <f>(MAX(E30-0.2,0))^2+(MAX(F30-0.75,0))^2+(MAX(G30-4,0))^2 +(MAX(H30-4,0))^2</f>
-        <v>0.77200000000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="11">
-        <v>3</v>
-      </c>
-      <c r="B31" s="11">
-        <v>3000</v>
-      </c>
-      <c r="C31" s="11">
-        <v>10</v>
-      </c>
-      <c r="D31" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="E31" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="F31" s="11">
-        <v>1.65</v>
-      </c>
-      <c r="G31" s="13">
-        <v>3.78</v>
-      </c>
-      <c r="H31" s="13">
-        <v>4.1900000000000004</v>
-      </c>
-      <c r="I31" s="13">
-        <f>(MAX(E31-0.2,0))^2+(MAX(F31-0.75,0))^2+(MAX(G31-4,0))^2 +(MAX(H31-4,0))^2</f>
-        <v>0.84609999999999996</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="12">
-        <v>3</v>
-      </c>
-      <c r="B32" s="12">
-        <v>3000</v>
-      </c>
-      <c r="C32" s="12">
-        <v>10</v>
-      </c>
-      <c r="D32" s="12">
-        <v>0.06</v>
-      </c>
-      <c r="E32" s="12">
-        <v>0.16</v>
-      </c>
-      <c r="F32" s="12">
+      <c r="F32" s="11">
         <v>1.71</v>
       </c>
       <c r="G32" s="10">
@@ -1457,48 +1460,103 @@
         <v>4.1900000000000004</v>
       </c>
       <c r="I32" s="10">
-        <f>(MAX(E32-0.2,0))^2+(MAX(F32-0.75,0))^2+(MAX(G32-4,0))^2 +(MAX(H32-4,0))^2</f>
-        <v>0.95770000000000011</v>
+        <f>SUM(E32:H32)+10*(MAX(E32-0.2,0))^2+10*(MAX(F32-0.75,0))^2+(MAX(G32-4,0))^2 +(MAX(H32-4,0))^2</f>
+        <v>19.082100000000001</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I33" s="13"/>
+      <c r="A33" s="12">
+        <v>3</v>
+      </c>
+      <c r="B33" s="12">
+        <v>2499.84284416015</v>
+      </c>
+      <c r="C33" s="12">
+        <v>8.4418355148223263</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0.29502416411524801</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0.2215944532707903</v>
+      </c>
+      <c r="F33" s="12">
+        <v>0.52705497119057965</v>
+      </c>
+      <c r="G33" s="12">
+        <v>4.0474031192403839</v>
+      </c>
+      <c r="H33" s="12">
+        <v>4.3329052486281219</v>
+      </c>
+      <c r="I33" s="14">
+        <f>SUM(E33:H33)+10*(MAX(E33-0.2,0))^2+10*(MAX(F33-0.75,0))^2+(MAX(G33-4,0))^2 +(MAX(H33-4,0))^2</f>
+        <v>9.2466939567283877</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I34" s="13"/>
+      <c r="A34" s="12">
+        <v>3</v>
+      </c>
+      <c r="B34" s="12">
+        <v>2499.84284416015</v>
+      </c>
+      <c r="C34" s="12">
+        <v>8.4418355148223263</v>
+      </c>
+      <c r="D34" s="12">
+        <v>0.29502416411524801</v>
+      </c>
+      <c r="E34" s="12">
+        <v>0.22346993607055199</v>
+      </c>
+      <c r="F34" s="12">
+        <v>0.54154839332437898</v>
+      </c>
+      <c r="G34" s="12">
+        <v>4.0435478968140428</v>
+      </c>
+      <c r="H34" s="12">
+        <v>4.3096978656593574</v>
+      </c>
+      <c r="I34" s="14">
+        <f>SUM(E34:H34)+10*(MAX(E34-0.2,0))^2+10*(MAX(F34-0.75,0))^2+(MAX(G34-4,0))^2 +(MAX(H34-4,0))^2</f>
+        <v>9.221581658170777</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I35" s="13"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I36" s="13"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I37" s="13"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I38" s="13"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I39" s="13"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>3</v>
-      </c>
-      <c r="B40">
-        <v>2999.6709384917081</v>
-      </c>
-      <c r="C40">
-        <v>9.1100693947327205</v>
-      </c>
-      <c r="D40">
-        <v>0.15038836079216389</v>
+      <c r="A35" s="12">
+        <v>3</v>
+      </c>
+      <c r="B35" s="12">
+        <v>2699.5652875355149</v>
+      </c>
+      <c r="C35" s="12">
+        <v>8.604142889770273</v>
+      </c>
+      <c r="D35" s="12">
+        <v>0.15992272527134241</v>
+      </c>
+      <c r="E35" s="12">
+        <v>0.20087401275955219</v>
+      </c>
+      <c r="F35" s="12">
+        <v>0.74189791660331306</v>
+      </c>
+      <c r="G35" s="12">
+        <v>4.0205571655092527</v>
+      </c>
+      <c r="H35" s="12">
+        <v>4.1419095495436471</v>
+      </c>
+      <c r="I35" s="14">
+        <f>SUM(E35:H35)+10*(MAX(E35-0.2,0))^2+10*(MAX(F35-0.75,0))^2+(MAX(G35-4,0))^2 +(MAX(H35-4,0))^2</f>
+        <v>9.1258072007042603</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I33">
-    <sortCondition ref="I2:I33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I32">
+    <sortCondition ref="I2:I32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1550,7 +1608,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2454,22 +2512,22 @@
       </c>
     </row>
     <row r="32" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="12">
-        <v>3</v>
-      </c>
-      <c r="B32" s="12">
-        <v>3000</v>
-      </c>
-      <c r="C32" s="12">
+      <c r="A32" s="11">
+        <v>3</v>
+      </c>
+      <c r="B32" s="11">
+        <v>3000</v>
+      </c>
+      <c r="C32" s="11">
         <v>10</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="11">
         <v>0.3</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="11">
         <v>0.15525102322819009</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F32" s="11">
         <v>0.53035584455315909</v>
       </c>
       <c r="G32" s="3">

</xml_diff>

<commit_message>
Update on all files
</commit_message>
<xml_diff>
--- a/Engineering_Optimization/Sim3_Results.xlsx
+++ b/Engineering_Optimization/Sim3_Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="false" showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="true"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,7 +11,7 @@
     <sheet name="LARGE_SET" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -42,7 +42,7 @@
     <font>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
+      <b val="true"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
@@ -68,7 +68,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.5999633777886288"/>
+        <fgColor theme="8" tint="0.59996337778863"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -80,49 +80,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.3999755851924192"/>
+        <fgColor theme="6" tint="0.39997558519242"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999511703848384"/>
+        <fgColor theme="4" tint="0.79995117038484"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999511703848384"/>
+        <fgColor theme="4" tint="0.79995117038484"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999511703848384"/>
+        <fgColor theme="4" tint="0.79995117038484"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999511703848384"/>
+        <fgColor theme="4" tint="0.79995117038484"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999511703848384"/>
+        <fgColor theme="4" tint="0.79995117038484"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999511703848384"/>
+        <fgColor theme="4" tint="0.79995117038484"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999511703848384"/>
+        <fgColor theme="4" tint="0.79995117038484"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -140,12 +140,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999511703848384"/>
+        <fgColor theme="4" tint="0.79995117038484"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -183,83 +183,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4"/>
   </cellStyleXfs>
-  <cellXfs count="50">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="51">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="false" pivotButton="false" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="false" pivotButton="false" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="false" pivotButton="false" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="2" xfId="0" quotePrefix="false" pivotButton="false" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="false" pivotButton="false" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="2" xfId="0" quotePrefix="false" pivotButton="false" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="0" xfId="0" quotePrefix="false" pivotButton="false" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="6" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="7" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="2" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="2" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="0" xfId="0" quotePrefix="false" pivotButton="false" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="1" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="8" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="2" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="2" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="2" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="4" fillId="8" borderId="2" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="2" fillId="8" borderId="0" xfId="0" quotePrefix="false" pivotButton="false" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="11" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="9" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="12" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="13" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="14" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="15" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="15" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="2" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="4" fillId="11" borderId="2" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="4" fillId="9" borderId="2" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="4" fillId="12" borderId="2" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="0" fillId="13" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="4" fillId="13" borderId="2" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="0" fillId="14" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="4" fillId="14" borderId="2" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="0" fillId="15" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="4" fillId="15" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="1" xfId="0" quotePrefix="false" pivotButton="false" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="15" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="4" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="3" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="4" fillId="15" borderId="2" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="2" fontId="4" fillId="11" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="false" pivotButton="false" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="false" pivotButton="false"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,29 +622,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="true" summaryRight="true"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="81" workbookViewId="0">
+    <sheetView tabSelected="true" topLeftCell="A59" zoomScale="81" workbookViewId="0">
       <selection activeCell="E102" sqref="A99:E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col width="18.1640625" bestFit="1" customWidth="1" style="15" min="1" max="1"/>
-    <col width="8.6640625" customWidth="1" style="15" min="2" max="2"/>
-    <col width="5.83203125" customWidth="1" style="15" min="3" max="3"/>
-    <col width="8.5" customWidth="1" style="15" min="4" max="4"/>
-    <col width="18.83203125" bestFit="1" customWidth="1" style="15" min="5" max="5"/>
-    <col width="18.5" bestFit="1" customWidth="1" style="15" min="6" max="6"/>
-    <col width="26.1640625" bestFit="1" customWidth="1" style="15" min="7" max="7"/>
-    <col width="31.6640625" bestFit="1" customWidth="1" style="15" min="8" max="8"/>
-    <col width="10.83203125" customWidth="1" style="15" min="9" max="9"/>
-    <col width="13.1640625" bestFit="1" customWidth="1" style="49" min="10" max="11"/>
+    <col min="1" max="1" width="18.140625" style="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" style="15" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" style="15" customWidth="true"/>
+    <col min="4" max="4" width="13.7109375" style="15" customWidth="true"/>
+    <col min="5" max="5" width="18.85546875" style="15" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="18.42578125" style="15" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="26.140625" style="15" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="31.7109375" style="15" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="10.83203125" style="15" customWidth="true"/>
+    <col min="10" max="11" width="13.1640625" style="49" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1652,7 +1654,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" ht="16" customHeight="1" s="49">
+    <row r="34" s="49" ht="16" customHeight="true">
       <c r="A34" s="18" t="n">
         <v>3</v>
       </c>
@@ -1712,7 +1714,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" ht="16" customHeight="1" s="49">
+    <row r="36" s="49" ht="16" customHeight="true">
       <c r="A36" s="18" t="n">
         <v>3</v>
       </c>
@@ -1742,7 +1744,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" ht="16" customHeight="1" s="49">
+    <row r="37" s="49" ht="16" customHeight="true">
       <c r="A37" s="18" t="n">
         <v>3</v>
       </c>
@@ -1832,7 +1834,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" ht="16" customHeight="1" s="49">
+    <row r="40" s="49" ht="16" customHeight="true">
       <c r="A40" s="18" t="n">
         <v>3</v>
       </c>
@@ -1952,7 +1954,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" ht="16" customHeight="1" s="49">
+    <row r="44" s="49" ht="16" customHeight="true">
       <c r="A44" s="16" t="n">
         <v>3</v>
       </c>
@@ -2042,7 +2044,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" ht="16" customHeight="1" s="49">
+    <row r="47" s="49" ht="16" customHeight="true">
       <c r="A47" s="16" t="n">
         <v>3</v>
       </c>
@@ -2102,7 +2104,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" ht="16" customHeight="1" s="49">
+    <row r="49" s="49" ht="16" customHeight="true">
       <c r="A49" s="27" t="n">
         <v>3</v>
       </c>
@@ -2192,7 +2194,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" ht="16" customHeight="1" s="49">
+    <row r="52" s="49" ht="16" customHeight="true">
       <c r="A52" s="16" t="n">
         <v>3</v>
       </c>
@@ -2702,7 +2704,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" ht="16" customHeight="1" s="49">
+    <row r="69" s="49" ht="16" customHeight="true">
       <c r="A69" s="13" t="n">
         <v>3</v>
       </c>
@@ -2732,7 +2734,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" ht="16" customHeight="1" s="49">
+    <row r="70" s="49" ht="16" customHeight="true">
       <c r="A70" s="13" t="n">
         <v>3</v>
       </c>
@@ -3448,34 +3450,290 @@
         <v>4.133083149698012</v>
       </c>
     </row>
-    <row r="101"/>
-    <row r="102"/>
+    <row r="94">
+      <c r="A94" s="15">
+        <v>3</v>
+      </c>
+      <c r="B94" s="15">
+        <v>2663.4008161824158</v>
+      </c>
+      <c r="C94" s="15">
+        <v>8.315735512168656</v>
+      </c>
+      <c r="D94" s="15">
+        <v>0.14817224060050621</v>
+      </c>
+      <c r="E94" s="15">
+        <v>0.20526986260054769</v>
+      </c>
+      <c r="F94" s="15">
+        <v>0.79276870693609069</v>
+      </c>
+      <c r="G94" s="15">
+        <v>4.0097725241772313</v>
+      </c>
+      <c r="H94" s="15">
+        <v>4.1397614984877285</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="15">
+        <v>3</v>
+      </c>
+      <c r="B95" s="15">
+        <v>2663.4008161824158</v>
+      </c>
+      <c r="C95" s="15">
+        <v>8.315735512168656</v>
+      </c>
+      <c r="D95" s="15">
+        <v>0.14817224060050621</v>
+      </c>
+      <c r="E95" s="15">
+        <v>0.20494446037981576</v>
+      </c>
+      <c r="F95" s="15">
+        <v>0.79522095377854196</v>
+      </c>
+      <c r="G95" s="15">
+        <v>4.0085410607660084</v>
+      </c>
+      <c r="H95" s="15">
+        <v>4.1390923046919328</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="15">
+        <v>3</v>
+      </c>
+      <c r="B96" s="15">
+        <v>2663.4248069444361</v>
+      </c>
+      <c r="C96" s="15">
+        <v>8.2962916316516555</v>
+      </c>
+      <c r="D96" s="15">
+        <v>0.054188570793946983</v>
+      </c>
+      <c r="E96" s="15">
+        <v>0.26027539899976648</v>
+      </c>
+      <c r="F96" s="15">
+        <v>1.8815943579961356</v>
+      </c>
+      <c r="G96" s="15">
+        <v>3.6950044727684053</v>
+      </c>
+      <c r="H96" s="15">
+        <v>4.172714263448583</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="15">
+        <v>3</v>
+      </c>
+      <c r="B97" s="15">
+        <v>2663.4008161824158</v>
+      </c>
+      <c r="C97" s="15">
+        <v>8.315735512168656</v>
+      </c>
+      <c r="D97" s="15">
+        <v>0.14817224060050621</v>
+      </c>
+      <c r="E97" s="15">
+        <v>0.20576912951205009</v>
+      </c>
+      <c r="F97" s="15">
+        <v>0.79404546237778906</v>
+      </c>
+      <c r="G97" s="15">
+        <v>4.0106381701099627</v>
+      </c>
+      <c r="H97" s="15">
+        <v>4.1410105287811518</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="15">
+        <v>3</v>
+      </c>
+      <c r="B98" s="15">
+        <v>2663.4248069444361</v>
+      </c>
+      <c r="C98" s="15">
+        <v>8.2962916316516555</v>
+      </c>
+      <c r="D98" s="15">
+        <v>0.054188570793946983</v>
+      </c>
+      <c r="E98" s="15">
+        <v>0.26034863258561064</v>
+      </c>
+      <c r="F98" s="15">
+        <v>1.8808320288048082</v>
+      </c>
+      <c r="G98" s="15">
+        <v>3.699408026113987</v>
+      </c>
+      <c r="H98" s="15">
+        <v>4.1711279392212584</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="15">
+        <v>3</v>
+      </c>
+      <c r="B99" s="15">
+        <v>2663.4008161824158</v>
+      </c>
+      <c r="C99" s="15">
+        <v>8.315735512168656</v>
+      </c>
+      <c r="D99" s="15">
+        <v>0.14817224060050621</v>
+      </c>
+      <c r="E99" s="15">
+        <v>0.16138842570052558</v>
+      </c>
+      <c r="F99" s="15">
+        <v>0.52196083588206843</v>
+      </c>
+      <c r="G99" s="15">
+        <v>7.9058881045504821</v>
+      </c>
+      <c r="H99" s="15">
+        <v>2.4319505654902307</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="15">
+        <v>3</v>
+      </c>
+      <c r="B100" s="15">
+        <v>2663.4248069444361</v>
+      </c>
+      <c r="C100" s="15">
+        <v>8.2962916316516555</v>
+      </c>
+      <c r="D100" s="15">
+        <v>0.054188570793946983</v>
+      </c>
+      <c r="E100" s="15">
+        <v>0.16138842570052558</v>
+      </c>
+      <c r="F100" s="15">
+        <v>0.52196083588206843</v>
+      </c>
+      <c r="G100" s="15">
+        <v>7.7399440257651548</v>
+      </c>
+      <c r="H100" s="15">
+        <v>1.9756661201547658</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="15">
+        <v>3</v>
+      </c>
+      <c r="B101" s="15">
+        <v>2663.4008161824158</v>
+      </c>
+      <c r="C101" s="15">
+        <v>8.315735512168656</v>
+      </c>
+      <c r="D101" s="15">
+        <v>0.14817224060050621</v>
+      </c>
+      <c r="E101" s="15">
+        <v>0.16138842570052558</v>
+      </c>
+      <c r="F101" s="15">
+        <v>0.52196083588206843</v>
+      </c>
+      <c r="G101" s="15">
+        <v>7.9058881045504821</v>
+      </c>
+      <c r="H101" s="15">
+        <v>2.4319505654902307</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="15">
+        <v>3</v>
+      </c>
+      <c r="B102" s="15">
+        <v>2663.4008161824158</v>
+      </c>
+      <c r="C102" s="15">
+        <v>8.315735512168656</v>
+      </c>
+      <c r="D102" s="15">
+        <v>0.14817224060050621</v>
+      </c>
+      <c r="E102" s="15">
+        <v>0.16138842570052558</v>
+      </c>
+      <c r="F102" s="15">
+        <v>0.52196083588206843</v>
+      </c>
+      <c r="G102" s="15">
+        <v>7.9058881045504821</v>
+      </c>
+      <c r="H102" s="15">
+        <v>2.4319505654902307</v>
+      </c>
+    </row>
     <row r="103">
-      <c r="A103" t="n">
-        <v>3</v>
-      </c>
-      <c r="B103" t="n">
-        <v>2663.400816182416</v>
-      </c>
-      <c r="C103" t="n">
-        <v>8.315735512168656</v>
-      </c>
-      <c r="D103" t="n">
-        <v>0.1481722406005062</v>
+      <c r="A103" s="0">
+        <v>3</v>
+      </c>
+      <c r="B103" s="0">
+        <v>2663.4248069444361</v>
+      </c>
+      <c r="C103" s="0">
+        <v>8.2962916316516555</v>
+      </c>
+      <c r="D103" s="0">
+        <v>0.054188570793946983</v>
+      </c>
+      <c r="E103" s="15">
+        <v>0.16138842570052558</v>
+      </c>
+      <c r="F103" s="15">
+        <v>0.52196083588206843</v>
+      </c>
+      <c r="G103" s="15">
+        <v>7.7399440257651548</v>
+      </c>
+      <c r="H103" s="15">
+        <v>1.9756661201547658</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="n">
-        <v>3</v>
-      </c>
-      <c r="B104" t="n">
-        <v>2663.424806944436</v>
-      </c>
-      <c r="C104" t="n">
-        <v>8.296291631651656</v>
-      </c>
-      <c r="D104" t="n">
-        <v>0.05418857079394698</v>
+      <c r="A104" s="0">
+        <v>3</v>
+      </c>
+      <c r="B104" s="0">
+        <v>2663.4248069444361</v>
+      </c>
+      <c r="C104" s="0">
+        <v>8.2962916316516555</v>
+      </c>
+      <c r="D104" s="0">
+        <v>0.054188570793946983</v>
+      </c>
+      <c r="E104" s="15">
+        <v>0.26241081030715102</v>
+      </c>
+      <c r="F104" s="15">
+        <v>1.873848616470764</v>
+      </c>
+      <c r="G104" s="15">
+        <v>3.6947726446762861</v>
+      </c>
+      <c r="H104" s="15">
+        <v>4.167661046723576</v>
       </c>
     </row>
   </sheetData>
@@ -3485,9 +3743,9 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="true" summaryRight="true"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:P6"/>
@@ -3498,7 +3756,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col width="10.83203125" customWidth="1" style="46" min="6" max="6"/>
+    <col min="6" max="6" width="10.83203125" style="46" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3793,9 +4051,9 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="true" summaryRight="true"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:I153"/>
@@ -3806,17 +4064,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col width="18.1640625" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
-    <col width="11.6640625" bestFit="1" customWidth="1" style="7" min="2" max="3"/>
-    <col width="12.6640625" customWidth="1" style="7" min="4" max="4"/>
-    <col width="18.83203125" bestFit="1" customWidth="1" style="7" min="5" max="5"/>
-    <col width="18.5" bestFit="1" customWidth="1" style="7" min="6" max="6"/>
-    <col width="26.1640625" bestFit="1" customWidth="1" style="7" min="7" max="7"/>
-    <col width="31.6640625" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
-    <col width="8.83203125" customWidth="1" style="7" min="9" max="9"/>
+    <col min="1" max="1" width="18.1640625" style="6" bestFit="true" customWidth="true"/>
+    <col min="2" max="3" width="11.6640625" style="7" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="12.6640625" style="7" customWidth="true"/>
+    <col min="5" max="5" width="18.83203125" style="7" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="18.5" style="7" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="26.1640625" style="7" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="31.6640625" style="7" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="8.83203125" style="7" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" s="49">
+    <row r="1" s="49" ht="15.75" customHeight="true">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Simulation Mode</t>
@@ -3863,7 +4121,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" s="49">
+    <row r="2" s="49" ht="15.75" customHeight="true">
       <c r="A2" s="5" t="n">
         <v>3</v>
       </c>
@@ -4763,7 +5021,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" customFormat="1" s="4">
+    <row r="32" s="4" customFormat="true">
       <c r="A32" s="9" t="n">
         <v>3</v>
       </c>

</xml_diff>